<commit_message>
LTC3: More Charger Controller BOM work.
Finally finished (hopefully).
</commit_message>
<xml_diff>
--- a/ltc3/bom/charge_controller/LTC3_Charge_Controller.xlsx
+++ b/ltc3/bom/charge_controller/LTC3_Charge_Controller.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="948" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="961" uniqueCount="342">
   <si>
     <t xml:space="preserve">Refs</t>
   </si>
@@ -58,6 +58,15 @@
     <t xml:space="preserve">-</t>
   </si>
   <si>
+    <t xml:space="preserve">Murata</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRM21BR71H184KA01L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">50V X7R 10%</t>
+  </si>
+  <si>
     <t xml:space="preserve">~</t>
   </si>
   <si>
@@ -70,6 +79,15 @@
     <t xml:space="preserve">0.1u</t>
   </si>
   <si>
+    <t xml:space="preserve">10V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRM21BR71E104KA01L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25V X7R 10%</t>
+  </si>
+  <si>
     <t xml:space="preserve">C1</t>
   </si>
   <si>
@@ -79,12 +97,6 @@
     <t xml:space="preserve">50V X7R</t>
   </si>
   <si>
-    <t xml:space="preserve">ceramic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Murata</t>
-  </si>
-  <si>
     <t xml:space="preserve">GRM21AR72A334KAC5L</t>
   </si>
   <si>
@@ -127,6 +139,21 @@
     <t xml:space="preserve">10u</t>
   </si>
   <si>
+    <t xml:space="preserve">75V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nichicon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UCD1K100MCL1GS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">alum. Electrolytic, 80V 20%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Capacitors_SMD:c_elec_6.3x7.7</t>
+  </si>
+  <si>
     <t xml:space="preserve">C35</t>
   </si>
   <si>
@@ -136,19 +163,10 @@
     <t xml:space="preserve">150u</t>
   </si>
   <si>
-    <t xml:space="preserve">75V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">aluminum electrolytic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nichicon</t>
-  </si>
-  <si>
     <t xml:space="preserve">UPW2A151MHD</t>
   </si>
   <si>
-    <t xml:space="preserve">100V 20%</t>
+    <t xml:space="preserve">alum. Electrolytic, 100V 20%</t>
   </si>
   <si>
     <t xml:space="preserve">Capacitors_ThroughHole:C_Radial_D12.5_L25_P5</t>
@@ -172,9 +190,18 @@
     <t xml:space="preserve">1u</t>
   </si>
   <si>
+    <t xml:space="preserve">GRM21BR71E105KA99K</t>
+  </si>
+  <si>
     <t xml:space="preserve">C30</t>
   </si>
   <si>
+    <t xml:space="preserve">GRJ21BC72A105KE11L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100V X7S 10%</t>
+  </si>
+  <si>
     <t xml:space="preserve">C9</t>
   </si>
   <si>
@@ -208,6 +235,9 @@
     <t xml:space="preserve">220n</t>
   </si>
   <si>
+    <t xml:space="preserve">GRM21BR71H224KA01L</t>
+  </si>
+  <si>
     <t xml:space="preserve">C15</t>
   </si>
   <si>
@@ -217,6 +247,12 @@
     <t xml:space="preserve">220p</t>
   </si>
   <si>
+    <t xml:space="preserve">Yago</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CC0805KRX7R9BB221</t>
+  </si>
+  <si>
     <t xml:space="preserve">C2</t>
   </si>
   <si>
@@ -229,9 +265,6 @@
     <t xml:space="preserve">UUX2A330MNL1GS</t>
   </si>
   <si>
-    <t xml:space="preserve">100V</t>
-  </si>
-  <si>
     <t xml:space="preserve">Capacitors_SMD:c_elec_10x10</t>
   </si>
   <si>
@@ -262,9 +295,6 @@
     <t xml:space="preserve">C24</t>
   </si>
   <si>
-    <t xml:space="preserve">10V</t>
-  </si>
-  <si>
     <t xml:space="preserve">C28</t>
   </si>
   <si>
@@ -283,6 +313,9 @@
     <t xml:space="preserve">470n</t>
   </si>
   <si>
+    <t xml:space="preserve">GRM21BR71H474KA88L</t>
+  </si>
+  <si>
     <t xml:space="preserve">C32</t>
   </si>
   <si>
@@ -292,10 +325,16 @@
     <t xml:space="preserve">68n</t>
   </si>
   <si>
+    <t xml:space="preserve">GRM219R71E683KA01D</t>
+  </si>
+  <si>
     <t xml:space="preserve">C16</t>
   </si>
   <si>
     <t xml:space="preserve">8.2n</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRM21BR71H823KA01L</t>
   </si>
   <si>
     <t xml:space="preserve">D1</t>
@@ -1016,7 +1055,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1053,12 +1092,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1110,7 +1143,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1120,14 +1153,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1151,19 +1176,20 @@
   <dimension ref="A1:I115"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B23" activeCellId="0" sqref="B23"/>
+      <selection pane="topLeft" activeCell="I11" activeCellId="0" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="5.46153846153846"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.9271255060729"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="10.0688259109312"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="10.1781376518219"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="16.497975708502"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="12.3198380566802"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="22.3886639676113"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="1" width="20.4615384615385"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="63.6275303643725"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="12.4251012145749"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="22.4939271255061"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="21.5101214574899"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="20.5668016194332"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="64.165991902834"/>
     <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -1210,1003 +1236,1042 @@
         <v>11</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>11</v>
+        <v>20</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="H7" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>11</v>
+        <v>41</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>13</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>11</v>
+        <v>41</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>13</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>39</v>
+        <v>11</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>40</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>11</v>
+        <v>56</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>11</v>
+        <v>58</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>59</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>11</v>
+        <v>71</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>11</v>
+        <v>71</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>11</v>
+        <v>75</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>11</v>
+        <v>76</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>65</v>
+        <v>77</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>66</v>
+        <v>78</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>39</v>
+        <v>11</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>40</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>68</v>
+        <v>80</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>71</v>
+        <v>82</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>66</v>
+        <v>78</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>39</v>
+        <v>11</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>40</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>68</v>
+        <v>80</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>66</v>
+        <v>78</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>39</v>
+        <v>11</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>40</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>68</v>
+        <v>80</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>78</v>
+        <v>89</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>80</v>
+        <v>19</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>11</v>
+        <v>97</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>11</v>
+        <v>97</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>89</v>
+        <v>100</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>11</v>
+        <v>101</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>90</v>
+        <v>102</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>91</v>
+        <v>103</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>11</v>
+        <v>104</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>92</v>
+        <v>105</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>93</v>
+        <v>106</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>11</v>
@@ -2215,24 +2280,24 @@
         <v>11</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>94</v>
+        <v>107</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>95</v>
+        <v>108</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>96</v>
+        <v>109</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>97</v>
+        <v>110</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>98</v>
+        <v>111</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>93</v>
+        <v>106</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>11</v>
@@ -2241,102 +2306,102 @@
         <v>11</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>94</v>
+        <v>107</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>95</v>
+        <v>108</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>96</v>
+        <v>109</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>97</v>
+        <v>110</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>99</v>
+        <v>112</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>100</v>
+        <v>113</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>102</v>
+        <v>115</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>103</v>
+        <v>116</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>105</v>
+        <v>118</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>106</v>
+        <v>119</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>107</v>
+        <v>120</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>108</v>
+        <v>121</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>102</v>
+        <v>115</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>109</v>
+        <v>122</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>105</v>
+        <v>118</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>111</v>
+        <v>124</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>112</v>
+        <v>125</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>113</v>
+        <v>126</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>114</v>
+        <v>127</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>115</v>
+        <v>128</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>116</v>
+        <v>129</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>97</v>
+        <v>110</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>117</v>
+        <v>130</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>118</v>
+        <v>131</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>11</v>
@@ -2345,24 +2410,24 @@
         <v>11</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>119</v>
+        <v>132</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>120</v>
+        <v>133</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>121</v>
+        <v>134</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>122</v>
+        <v>135</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>123</v>
+        <v>136</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>124</v>
+        <v>137</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>11</v>
@@ -2371,76 +2436,76 @@
         <v>11</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>125</v>
+        <v>138</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>126</v>
+        <v>139</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>127</v>
+        <v>140</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>128</v>
+        <v>141</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>129</v>
+        <v>142</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>130</v>
+        <v>143</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>131</v>
+        <v>144</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>132</v>
+        <v>145</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>133</v>
+        <v>146</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>134</v>
+        <v>147</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>135</v>
+        <v>148</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>136</v>
+        <v>149</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>130</v>
+        <v>143</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>137</v>
+        <v>150</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>132</v>
+        <v>145</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>133</v>
+        <v>146</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>134</v>
+        <v>147</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>138</v>
+        <v>151</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>139</v>
+        <v>152</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>140</v>
+        <v>153</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>11</v>
@@ -2452,21 +2517,21 @@
         <v>11</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>141</v>
+        <v>154</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>142</v>
+        <v>155</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>143</v>
+        <v>156</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>144</v>
+        <v>157</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>130</v>
+        <v>143</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>11</v>
@@ -2475,50 +2540,50 @@
         <v>11</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>132</v>
+        <v>145</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>133</v>
+        <v>146</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>134</v>
+        <v>147</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>138</v>
+        <v>151</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>145</v>
+        <v>158</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>140</v>
+        <v>153</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>146</v>
+        <v>159</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>147</v>
+        <v>160</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>141</v>
+        <v>154</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>142</v>
+        <v>155</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>143</v>
+        <v>156</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>148</v>
+        <v>161</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>140</v>
+        <v>153</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>11</v>
@@ -2527,24 +2592,24 @@
         <v>11</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>147</v>
+        <v>160</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>149</v>
+        <v>162</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>142</v>
+        <v>155</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>150</v>
+        <v>163</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>151</v>
+        <v>164</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>152</v>
+        <v>165</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>11</v>
@@ -2553,24 +2618,24 @@
         <v>11</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>153</v>
+        <v>166</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>154</v>
+        <v>167</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>155</v>
+        <v>168</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>156</v>
+        <v>169</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>157</v>
+        <v>170</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>158</v>
+        <v>171</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>11</v>
@@ -2579,24 +2644,24 @@
         <v>11</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>159</v>
+        <v>172</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>158</v>
+        <v>171</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>160</v>
+        <v>173</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>161</v>
+        <v>174</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
-        <v>162</v>
+        <v>175</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>158</v>
+        <v>171</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>11</v>
@@ -2605,24 +2670,24 @@
         <v>11</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>159</v>
+        <v>172</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>158</v>
+        <v>171</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>160</v>
+        <v>173</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>161</v>
+        <v>174</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>163</v>
+        <v>176</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>158</v>
+        <v>171</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>11</v>
@@ -2631,24 +2696,24 @@
         <v>11</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>159</v>
+        <v>172</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>158</v>
+        <v>171</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>160</v>
+        <v>173</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>161</v>
+        <v>174</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
-        <v>164</v>
+        <v>177</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>158</v>
+        <v>171</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>11</v>
@@ -2657,24 +2722,24 @@
         <v>11</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>159</v>
+        <v>172</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>158</v>
+        <v>171</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>160</v>
+        <v>173</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>161</v>
+        <v>174</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
-        <v>165</v>
+        <v>178</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>166</v>
+        <v>179</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>11</v>
@@ -2683,24 +2748,24 @@
         <v>11</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>114</v>
+        <v>127</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>167</v>
+        <v>180</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>168</v>
+        <v>181</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>169</v>
+        <v>182</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>170</v>
+        <v>183</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>171</v>
+        <v>184</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>11</v>
@@ -2709,76 +2774,76 @@
         <v>11</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>172</v>
+        <v>185</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>173</v>
+        <v>186</v>
       </c>
       <c r="H57" s="1" t="s">
-        <v>174</v>
+        <v>187</v>
       </c>
       <c r="I57" s="1" t="s">
-        <v>169</v>
+        <v>182</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>175</v>
+        <v>188</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>176</v>
+        <v>189</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>177</v>
+        <v>190</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>178</v>
+        <v>191</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>179</v>
+        <v>192</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>180</v>
+        <v>193</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>181</v>
+        <v>194</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>182</v>
+        <v>195</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>177</v>
+        <v>190</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>178</v>
+        <v>191</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>183</v>
+        <v>196</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I59" s="1" t="s">
-        <v>180</v>
+        <v>193</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>184</v>
+        <v>197</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>185</v>
+        <v>198</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>11</v>
@@ -2787,24 +2852,24 @@
         <v>11</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>178</v>
+        <v>191</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>186</v>
+        <v>199</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I60" s="1" t="s">
-        <v>180</v>
+        <v>193</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
-        <v>187</v>
+        <v>200</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>185</v>
+        <v>198</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>11</v>
@@ -2813,24 +2878,24 @@
         <v>11</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>178</v>
+        <v>191</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>186</v>
+        <v>199</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I61" s="1" t="s">
-        <v>180</v>
+        <v>193</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>188</v>
+        <v>201</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>189</v>
+        <v>202</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>11</v>
@@ -2839,24 +2904,24 @@
         <v>11</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>178</v>
+        <v>191</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>190</v>
+        <v>203</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I62" s="1" t="s">
-        <v>191</v>
+        <v>204</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
-        <v>192</v>
+        <v>205</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>189</v>
+        <v>202</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>11</v>
@@ -2865,50 +2930,50 @@
         <v>11</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>178</v>
+        <v>191</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>190</v>
+        <v>203</v>
       </c>
       <c r="H63" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I63" s="1" t="s">
-        <v>191</v>
+        <v>204</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="H64" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I64" s="1" t="s">
         <v>193</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D64" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E64" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="F64" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="H64" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I64" s="1" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
-        <v>196</v>
+        <v>209</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>197</v>
+        <v>210</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>11</v>
@@ -2917,76 +2982,76 @@
         <v>11</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>178</v>
+        <v>191</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>198</v>
+        <v>211</v>
       </c>
       <c r="H65" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I65" s="1" t="s">
-        <v>180</v>
+        <v>193</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
-        <v>199</v>
+        <v>212</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>200</v>
+        <v>213</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>177</v>
+        <v>190</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>178</v>
+        <v>191</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>201</v>
+        <v>214</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I66" s="1" t="s">
-        <v>180</v>
+        <v>193</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
-        <v>202</v>
+        <v>215</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>203</v>
+        <v>216</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>177</v>
+        <v>190</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>204</v>
+        <v>217</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>205</v>
+        <v>218</v>
       </c>
       <c r="H67" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I67" s="1" t="s">
-        <v>180</v>
+        <v>193</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
-        <v>206</v>
+        <v>219</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>207</v>
+        <v>220</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>11</v>
@@ -2995,24 +3060,24 @@
         <v>11</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>178</v>
+        <v>191</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>208</v>
+        <v>221</v>
       </c>
       <c r="H68" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I68" s="1" t="s">
-        <v>180</v>
+        <v>193</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
-        <v>209</v>
+        <v>222</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>210</v>
+        <v>223</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>11</v>
@@ -3021,24 +3086,24 @@
         <v>11</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>178</v>
+        <v>191</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>211</v>
+        <v>224</v>
       </c>
       <c r="H69" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I69" s="1" t="s">
-        <v>180</v>
+        <v>193</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
-        <v>212</v>
+        <v>225</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>213</v>
+        <v>226</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>11</v>
@@ -3047,24 +3112,24 @@
         <v>11</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>178</v>
+        <v>191</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>214</v>
+        <v>227</v>
       </c>
       <c r="H70" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I70" s="1" t="s">
-        <v>180</v>
+        <v>193</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
-        <v>215</v>
+        <v>228</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>216</v>
+        <v>229</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>11</v>
@@ -3073,24 +3138,24 @@
         <v>11</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>178</v>
+        <v>191</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>217</v>
+        <v>230</v>
       </c>
       <c r="H71" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I71" s="1" t="s">
-        <v>180</v>
+        <v>193</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
-        <v>218</v>
+        <v>231</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>189</v>
+        <v>202</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>11</v>
@@ -3099,24 +3164,24 @@
         <v>11</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>178</v>
+        <v>191</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>190</v>
+        <v>203</v>
       </c>
       <c r="H72" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I72" s="1" t="s">
-        <v>191</v>
+        <v>204</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
-        <v>219</v>
+        <v>232</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>220</v>
+        <v>233</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>11</v>
@@ -3125,24 +3190,24 @@
         <v>11</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>221</v>
+        <v>234</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>222</v>
+        <v>235</v>
       </c>
       <c r="H73" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I73" s="1" t="s">
-        <v>180</v>
+        <v>193</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="s">
-        <v>223</v>
+        <v>236</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>224</v>
+        <v>237</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>11</v>
@@ -3151,24 +3216,24 @@
         <v>11</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>178</v>
+        <v>191</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>225</v>
+        <v>238</v>
       </c>
       <c r="H74" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I74" s="1" t="s">
-        <v>180</v>
+        <v>193</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="s">
-        <v>226</v>
+        <v>239</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>227</v>
+        <v>240</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>11</v>
@@ -3177,24 +3242,24 @@
         <v>11</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>178</v>
+        <v>191</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>228</v>
+        <v>241</v>
       </c>
       <c r="H75" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I75" s="1" t="s">
-        <v>180</v>
+        <v>193</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="s">
-        <v>229</v>
+        <v>242</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>185</v>
+        <v>198</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>11</v>
@@ -3203,53 +3268,53 @@
         <v>11</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>178</v>
+        <v>191</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>186</v>
+        <v>199</v>
       </c>
       <c r="H76" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I76" s="1" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="77" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="B77" s="3" t="s">
-        <v>231</v>
-      </c>
-      <c r="C77" s="3" t="s">
-        <v>232</v>
-      </c>
-      <c r="D77" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E77" s="3" t="s">
-        <v>233</v>
-      </c>
-      <c r="F77" s="4" t="s">
-        <v>234</v>
-      </c>
-      <c r="G77" s="3" t="s">
-        <v>235</v>
-      </c>
-      <c r="H77" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I77" s="3" t="s">
-        <v>236</v>
+        <v>193</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="G77" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="H77" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I77" s="1" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="s">
-        <v>237</v>
+        <v>250</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>238</v>
+        <v>251</v>
       </c>
       <c r="C78" s="1" t="s">
         <v>11</v>
@@ -3258,24 +3323,24 @@
         <v>11</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>178</v>
+        <v>191</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>239</v>
+        <v>252</v>
       </c>
       <c r="H78" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I78" s="1" t="s">
-        <v>180</v>
+        <v>193</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="s">
-        <v>240</v>
+        <v>253</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>241</v>
+        <v>254</v>
       </c>
       <c r="C79" s="1" t="s">
         <v>11</v>
@@ -3284,76 +3349,76 @@
         <v>11</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>178</v>
+        <v>191</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>242</v>
+        <v>255</v>
       </c>
       <c r="H79" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I79" s="1" t="s">
-        <v>180</v>
+        <v>193</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="s">
-        <v>243</v>
+        <v>256</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>244</v>
+        <v>257</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>245</v>
+        <v>258</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>178</v>
+        <v>191</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>246</v>
+        <v>259</v>
       </c>
       <c r="H80" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I80" s="1" t="s">
-        <v>180</v>
+        <v>193</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="1" t="s">
-        <v>247</v>
+        <v>260</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>244</v>
+        <v>257</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>248</v>
+        <v>261</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>178</v>
+        <v>191</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>246</v>
+        <v>259</v>
       </c>
       <c r="H81" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I81" s="1" t="s">
-        <v>180</v>
+        <v>193</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="1" t="s">
-        <v>249</v>
+        <v>262</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>189</v>
+        <v>202</v>
       </c>
       <c r="C82" s="1" t="s">
         <v>11</v>
@@ -3362,76 +3427,76 @@
         <v>11</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>178</v>
+        <v>191</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>190</v>
+        <v>203</v>
       </c>
       <c r="H82" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I82" s="1" t="s">
-        <v>191</v>
+        <v>204</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="1" t="s">
-        <v>250</v>
+        <v>263</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>251</v>
+        <v>264</v>
       </c>
       <c r="C83" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>252</v>
+        <v>265</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>178</v>
+        <v>191</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>253</v>
+        <v>266</v>
       </c>
       <c r="H83" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I83" s="1" t="s">
-        <v>180</v>
+        <v>193</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="1" t="s">
-        <v>254</v>
+        <v>267</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>210</v>
+        <v>223</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>255</v>
+        <v>268</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>178</v>
+        <v>191</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>211</v>
+        <v>224</v>
       </c>
       <c r="H84" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I84" s="1" t="s">
-        <v>180</v>
+        <v>193</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="1" t="s">
-        <v>256</v>
+        <v>269</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>238</v>
+        <v>251</v>
       </c>
       <c r="C85" s="1" t="s">
         <v>11</v>
@@ -3440,24 +3505,24 @@
         <v>11</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>178</v>
+        <v>191</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>239</v>
+        <v>252</v>
       </c>
       <c r="H85" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I85" s="1" t="s">
-        <v>180</v>
+        <v>193</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="1" t="s">
-        <v>257</v>
+        <v>270</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>238</v>
+        <v>251</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>11</v>
@@ -3466,24 +3531,24 @@
         <v>11</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>178</v>
+        <v>191</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>239</v>
+        <v>252</v>
       </c>
       <c r="H86" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I86" s="1" t="s">
-        <v>180</v>
+        <v>193</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="1" t="s">
-        <v>258</v>
+        <v>271</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>259</v>
+        <v>272</v>
       </c>
       <c r="C87" s="1" t="s">
         <v>11</v>
@@ -3492,53 +3557,53 @@
         <v>11</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>178</v>
+        <v>191</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>260</v>
+        <v>273</v>
       </c>
       <c r="H87" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I87" s="1" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="88" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="3" t="s">
-        <v>261</v>
-      </c>
-      <c r="B88" s="3" t="s">
-        <v>231</v>
-      </c>
-      <c r="C88" s="4" t="s">
-        <v>232</v>
-      </c>
-      <c r="D88" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E88" s="3" t="s">
-        <v>233</v>
-      </c>
-      <c r="F88" s="4" t="s">
-        <v>234</v>
-      </c>
-      <c r="G88" s="3" t="s">
-        <v>235</v>
-      </c>
-      <c r="H88" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I88" s="3" t="s">
-        <v>236</v>
+        <v>193</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E88" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="F88" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="G88" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="H88" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I88" s="1" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="1" t="s">
-        <v>262</v>
+        <v>275</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>263</v>
+        <v>276</v>
       </c>
       <c r="C89" s="1" t="s">
         <v>11</v>
@@ -3547,50 +3612,50 @@
         <v>11</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>178</v>
+        <v>191</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>264</v>
+        <v>277</v>
       </c>
       <c r="H89" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I89" s="1" t="s">
-        <v>180</v>
+        <v>193</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="1" t="s">
-        <v>265</v>
+        <v>278</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>263</v>
+        <v>276</v>
       </c>
       <c r="C90" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>266</v>
+        <v>279</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>178</v>
+        <v>191</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>264</v>
+        <v>277</v>
       </c>
       <c r="H90" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I90" s="1" t="s">
-        <v>180</v>
+        <v>193</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="1" t="s">
-        <v>267</v>
+        <v>280</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>189</v>
+        <v>202</v>
       </c>
       <c r="C91" s="1" t="s">
         <v>11</v>
@@ -3599,131 +3664,131 @@
         <v>11</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>178</v>
+        <v>191</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>268</v>
+        <v>281</v>
       </c>
       <c r="H91" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I91" s="1" t="s">
-        <v>191</v>
+        <v>204</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="1" t="s">
-        <v>269</v>
+        <v>282</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>270</v>
+        <v>283</v>
       </c>
       <c r="C92" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>271</v>
+        <v>284</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>178</v>
+        <v>191</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>272</v>
+        <v>285</v>
       </c>
       <c r="H92" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I92" s="1" t="s">
-        <v>180</v>
+        <v>193</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="1" t="s">
-        <v>273</v>
+        <v>286</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>274</v>
+        <v>287</v>
       </c>
       <c r="C93" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>275</v>
+        <v>288</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>178</v>
+        <v>191</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>276</v>
+        <v>289</v>
       </c>
       <c r="H93" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I93" s="1" t="s">
-        <v>180</v>
+        <v>193</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="1" t="s">
-        <v>277</v>
+        <v>290</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>278</v>
+        <v>291</v>
       </c>
       <c r="C94" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>279</v>
+        <v>292</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>178</v>
+        <v>191</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>280</v>
+        <v>293</v>
       </c>
       <c r="H94" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I94" s="1" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="95" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="3" t="s">
-        <v>281</v>
-      </c>
-      <c r="B95" s="3" t="s">
-        <v>231</v>
-      </c>
-      <c r="C95" s="3" t="s">
-        <v>232</v>
-      </c>
-      <c r="D95" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E95" s="3" t="s">
-        <v>233</v>
-      </c>
-      <c r="F95" s="4" t="s">
-        <v>234</v>
-      </c>
-      <c r="G95" s="3" t="s">
-        <v>235</v>
-      </c>
-      <c r="H95" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I95" s="3" t="s">
-        <v>236</v>
+        <v>193</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E95" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="F95" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="G95" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="H95" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I95" s="1" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="1" t="s">
-        <v>282</v>
+        <v>295</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>238</v>
+        <v>251</v>
       </c>
       <c r="C96" s="1" t="s">
         <v>11</v>
@@ -3732,105 +3797,105 @@
         <v>11</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>178</v>
+        <v>191</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>239</v>
+        <v>252</v>
       </c>
       <c r="H96" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I96" s="1" t="s">
-        <v>180</v>
+        <v>193</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="1" t="s">
-        <v>283</v>
+        <v>296</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>284</v>
+        <v>297</v>
       </c>
       <c r="C97" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>285</v>
+        <v>298</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>178</v>
+        <v>191</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>286</v>
+        <v>299</v>
       </c>
       <c r="H97" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I97" s="1" t="s">
-        <v>180</v>
+        <v>193</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="1" t="s">
-        <v>287</v>
+        <v>300</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>288</v>
+        <v>301</v>
       </c>
       <c r="C98" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>289</v>
+        <v>302</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>178</v>
+        <v>191</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>290</v>
+        <v>303</v>
       </c>
       <c r="H98" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I98" s="1" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="99" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="3" t="s">
-        <v>291</v>
-      </c>
-      <c r="B99" s="3" t="s">
-        <v>292</v>
-      </c>
-      <c r="C99" s="3" t="s">
-        <v>235</v>
-      </c>
-      <c r="D99" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E99" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="F99" s="3" t="s">
-        <v>293</v>
-      </c>
-      <c r="G99" s="3" t="s">
-        <v>235</v>
-      </c>
-      <c r="H99" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I99" s="3" t="s">
-        <v>294</v>
+        <v>193</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="D99" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E99" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="F99" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="G99" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="H99" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I99" s="1" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="1" t="s">
-        <v>295</v>
+        <v>308</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>296</v>
+        <v>309</v>
       </c>
       <c r="C100" s="1" t="s">
         <v>11</v>
@@ -3839,24 +3904,24 @@
         <v>11</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>297</v>
+        <v>310</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>298</v>
+        <v>311</v>
       </c>
       <c r="H100" s="1" t="s">
-        <v>299</v>
+        <v>312</v>
       </c>
       <c r="I100" s="1" t="s">
-        <v>300</v>
+        <v>313</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="1" t="s">
-        <v>301</v>
+        <v>314</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>296</v>
+        <v>309</v>
       </c>
       <c r="C101" s="1" t="s">
         <v>11</v>
@@ -3865,24 +3930,24 @@
         <v>11</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>297</v>
+        <v>310</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>298</v>
+        <v>311</v>
       </c>
       <c r="H101" s="1" t="s">
-        <v>299</v>
+        <v>312</v>
       </c>
       <c r="I101" s="1" t="s">
-        <v>300</v>
+        <v>313</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="1" t="s">
-        <v>302</v>
+        <v>315</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>303</v>
+        <v>316</v>
       </c>
       <c r="C102" s="1" t="s">
         <v>11</v>
@@ -3891,24 +3956,24 @@
         <v>11</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>304</v>
+        <v>317</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>305</v>
+        <v>318</v>
       </c>
       <c r="H102" s="1" t="s">
-        <v>306</v>
+        <v>319</v>
       </c>
       <c r="I102" s="1" t="s">
-        <v>307</v>
+        <v>320</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="1" t="s">
-        <v>308</v>
+        <v>321</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>309</v>
+        <v>322</v>
       </c>
       <c r="C103" s="1" t="s">
         <v>11</v>
@@ -3917,24 +3982,24 @@
         <v>11</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>304</v>
+        <v>317</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>310</v>
+        <v>323</v>
       </c>
       <c r="H103" s="1" t="s">
-        <v>311</v>
+        <v>324</v>
       </c>
       <c r="I103" s="1" t="s">
-        <v>312</v>
+        <v>325</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="1" t="s">
-        <v>313</v>
+        <v>326</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>314</v>
+        <v>327</v>
       </c>
       <c r="C104" s="1" t="s">
         <v>11</v>
@@ -3949,18 +4014,18 @@
         <v>11</v>
       </c>
       <c r="H104" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I104" s="1" t="s">
-        <v>315</v>
+        <v>328</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="1" t="s">
-        <v>316</v>
+        <v>329</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>314</v>
+        <v>327</v>
       </c>
       <c r="C105" s="1" t="s">
         <v>11</v>
@@ -3975,18 +4040,18 @@
         <v>11</v>
       </c>
       <c r="H105" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I105" s="1" t="s">
-        <v>315</v>
+        <v>328</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="1" t="s">
-        <v>317</v>
+        <v>330</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>314</v>
+        <v>327</v>
       </c>
       <c r="C106" s="1" t="s">
         <v>11</v>
@@ -4001,18 +4066,18 @@
         <v>11</v>
       </c>
       <c r="H106" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I106" s="1" t="s">
-        <v>315</v>
+        <v>328</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="1" t="s">
-        <v>318</v>
+        <v>331</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>314</v>
+        <v>327</v>
       </c>
       <c r="C107" s="1" t="s">
         <v>11</v>
@@ -4027,18 +4092,18 @@
         <v>11</v>
       </c>
       <c r="H107" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I107" s="1" t="s">
-        <v>315</v>
+        <v>328</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="1" t="s">
-        <v>319</v>
+        <v>332</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>314</v>
+        <v>327</v>
       </c>
       <c r="C108" s="1" t="s">
         <v>11</v>
@@ -4053,18 +4118,18 @@
         <v>11</v>
       </c>
       <c r="H108" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I108" s="1" t="s">
-        <v>315</v>
+        <v>328</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="1" t="s">
-        <v>320</v>
+        <v>333</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>314</v>
+        <v>327</v>
       </c>
       <c r="C109" s="1" t="s">
         <v>11</v>
@@ -4079,18 +4144,18 @@
         <v>11</v>
       </c>
       <c r="H109" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I109" s="1" t="s">
-        <v>315</v>
+        <v>328</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="1" t="s">
-        <v>321</v>
+        <v>334</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>322</v>
+        <v>335</v>
       </c>
       <c r="C110" s="1" t="s">
         <v>11</v>
@@ -4105,18 +4170,18 @@
         <v>11</v>
       </c>
       <c r="H110" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I110" s="1" t="s">
-        <v>323</v>
+        <v>336</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="1" t="s">
-        <v>324</v>
+        <v>337</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>322</v>
+        <v>335</v>
       </c>
       <c r="C111" s="1" t="s">
         <v>11</v>
@@ -4131,18 +4196,18 @@
         <v>11</v>
       </c>
       <c r="H111" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I111" s="1" t="s">
-        <v>323</v>
+        <v>336</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="1" t="s">
-        <v>325</v>
+        <v>338</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>322</v>
+        <v>335</v>
       </c>
       <c r="C112" s="1" t="s">
         <v>11</v>
@@ -4157,18 +4222,18 @@
         <v>11</v>
       </c>
       <c r="H112" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I112" s="1" t="s">
-        <v>323</v>
+        <v>336</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="1" t="s">
-        <v>326</v>
+        <v>339</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>322</v>
+        <v>335</v>
       </c>
       <c r="C113" s="1" t="s">
         <v>11</v>
@@ -4183,19 +4248,19 @@
         <v>11</v>
       </c>
       <c r="H113" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I113" s="1" t="s">
-        <v>323</v>
+        <v>336</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="B114" s="1" t="s">
         <v>327</v>
       </c>
-      <c r="B114" s="1" t="s">
-        <v>314</v>
-      </c>
       <c r="C114" s="1" t="s">
         <v>11</v>
       </c>
@@ -4209,36 +4274,36 @@
         <v>11</v>
       </c>
       <c r="H114" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I114" s="1" t="s">
-        <v>315</v>
+        <v>328</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D115" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E115" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F115" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H115" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I115" s="1" t="s">
         <v>328</v>
-      </c>
-      <c r="B115" s="1" t="s">
-        <v>314</v>
-      </c>
-      <c r="C115" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D115" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E115" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F115" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H115" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I115" s="1" t="s">
-        <v>315</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
LTC3: Corrected charge controller shunt resistor BOM data.
Really done this time, for reals.
</commit_message>
<xml_diff>
--- a/ltc3/bom/charge_controller/LTC3_Charge_Controller.xlsx
+++ b/ltc3/bom/charge_controller/LTC3_Charge_Controller.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1007" uniqueCount="357">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1011" uniqueCount="358">
   <si>
     <t xml:space="preserve">Refs</t>
   </si>
@@ -634,6 +634,9 @@
     <t xml:space="preserve">RC0805FR-0710KL</t>
   </si>
   <si>
+    <t xml:space="preserve">1% 1/8W</t>
+  </si>
+  <si>
     <t xml:space="preserve">R4</t>
   </si>
   <si>
@@ -778,13 +781,10 @@
     <t xml:space="preserve">1% 1W</t>
   </si>
   <si>
-    <t xml:space="preserve">Bourns</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CST0612-FC-R0015E</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Resistors_SMD:R_2512</t>
+    <t xml:space="preserve">WSLP1206R0100FEA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resistors_SMD:R_1206</t>
   </si>
   <si>
     <t xml:space="preserve">R21</t>
@@ -865,10 +865,10 @@
     <t xml:space="preserve">5m</t>
   </si>
   <si>
-    <t xml:space="preserve">1% 1/8W</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Resistors_SMD:R_1210_HandSoldering</t>
+    <t xml:space="preserve">WSL12065L000FEA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1% 1/4W</t>
   </si>
   <si>
     <t xml:space="preserve">R32</t>
@@ -964,7 +964,10 @@
     <t xml:space="preserve">100m</t>
   </si>
   <si>
-    <t xml:space="preserve">RL2512FK-070R1L</t>
+    <t xml:space="preserve">Samsung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RUW3216FR100CS</t>
   </si>
   <si>
     <t xml:space="preserve">R43</t>
@@ -1188,7 +1191,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1198,6 +1201,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1220,8 +1227,8 @@
   </sheetPr>
   <dimension ref="A1:I120"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A52" activeCellId="0" sqref="A52"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A72" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H98" activeCellId="0" sqref="H98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1230,11 +1237,11 @@
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.9271255060729"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="1" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="16.497975708502"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="12.6396761133603"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="22.7085020242915"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="21.9595141700405"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="20.7813765182186"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="65.2348178137652"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="12.748987854251"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="22.8178137651822"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="22.1740890688259"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="20.8866396761134"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="65.7692307692308"/>
     <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -2928,6 +2935,9 @@
       <c r="F61" s="1" t="s">
         <v>203</v>
       </c>
+      <c r="G61" s="1" t="s">
+        <v>204</v>
+      </c>
       <c r="H61" s="1" t="s">
         <v>16</v>
       </c>
@@ -2937,7 +2947,7 @@
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>202</v>
@@ -2954,6 +2964,9 @@
       <c r="F62" s="1" t="s">
         <v>203</v>
       </c>
+      <c r="G62" s="1" t="s">
+        <v>204</v>
+      </c>
       <c r="H62" s="1" t="s">
         <v>16</v>
       </c>
@@ -2963,10 +2976,10 @@
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>12</v>
@@ -2978,10 +2991,10 @@
         <v>195</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="H63" s="1" t="s">
         <v>16</v>
@@ -2992,10 +3005,10 @@
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>12</v>
@@ -3007,10 +3020,10 @@
         <v>195</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="H64" s="1" t="s">
         <v>16</v>
@@ -3021,10 +3034,10 @@
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>12</v>
@@ -3036,7 +3049,7 @@
         <v>195</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="H65" s="1" t="s">
         <v>16</v>
@@ -3047,10 +3060,10 @@
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>12</v>
@@ -3062,7 +3075,7 @@
         <v>195</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="H66" s="1" t="s">
         <v>16</v>
@@ -3073,10 +3086,10 @@
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>194</v>
@@ -3088,7 +3101,7 @@
         <v>195</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="H67" s="1" t="s">
         <v>16</v>
@@ -3097,38 +3110,38 @@
         <v>197</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A68" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="B68" s="1" t="s">
+    <row r="68" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A68" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="C68" s="1" t="s">
+      <c r="B68" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="C68" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="D68" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E68" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="F68" s="1" t="s">
+      <c r="D68" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E68" s="3" t="s">
         <v>222</v>
       </c>
-      <c r="H68" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I68" s="1" t="s">
+      <c r="F68" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="H68" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I68" s="3" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>12</v>
@@ -3140,7 +3153,7 @@
         <v>195</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="H69" s="1" t="s">
         <v>16</v>
@@ -3151,10 +3164,10 @@
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>12</v>
@@ -3166,7 +3179,7 @@
         <v>195</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="H70" s="1" t="s">
         <v>16</v>
@@ -3177,10 +3190,10 @@
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>12</v>
@@ -3192,7 +3205,7 @@
         <v>195</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="H71" s="1" t="s">
         <v>16</v>
@@ -3203,10 +3216,10 @@
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>12</v>
@@ -3218,7 +3231,7 @@
         <v>195</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="H72" s="1" t="s">
         <v>16</v>
@@ -3229,10 +3242,10 @@
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>12</v>
@@ -3244,21 +3257,21 @@
         <v>195</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="H73" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I73" s="1" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>12</v>
@@ -3267,10 +3280,10 @@
         <v>12</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="H74" s="1" t="s">
         <v>16</v>
@@ -3281,10 +3294,10 @@
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>12</v>
@@ -3296,7 +3309,7 @@
         <v>195</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="H75" s="1" t="s">
         <v>16</v>
@@ -3305,12 +3318,12 @@
         <v>197</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="13.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>12</v>
@@ -3322,7 +3335,7 @@
         <v>195</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="H76" s="1" t="s">
         <v>16</v>
@@ -3333,7 +3346,7 @@
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>202</v>
@@ -3350,6 +3363,9 @@
       <c r="F77" s="1" t="s">
         <v>203</v>
       </c>
+      <c r="G77" s="1" t="s">
+        <v>204</v>
+      </c>
       <c r="H77" s="1" t="s">
         <v>16</v>
       </c>
@@ -3357,58 +3373,58 @@
         <v>197</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A78" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="B78" s="1" t="s">
+    <row r="78" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A78" s="3" t="s">
         <v>250</v>
       </c>
-      <c r="C78" s="1" t="s">
+      <c r="B78" s="3" t="s">
         <v>251</v>
       </c>
-      <c r="D78" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E78" s="1" t="s">
+      <c r="C78" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="F78" s="1" t="s">
+      <c r="D78" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E78" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="F78" s="3" t="s">
         <v>253</v>
       </c>
-      <c r="G78" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="H78" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I78" s="1" t="s">
+      <c r="G78" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="H78" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I78" s="3" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A79" s="1" t="s">
+    <row r="79" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A79" s="3" t="s">
         <v>255</v>
       </c>
-      <c r="B79" s="1" t="s">
+      <c r="B79" s="3" t="s">
         <v>256</v>
       </c>
-      <c r="C79" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D79" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E79" s="1" t="s">
+      <c r="C79" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D79" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E79" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="F79" s="1" t="s">
+      <c r="F79" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="H79" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I79" s="1" t="s">
+      <c r="H79" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I79" s="3" t="s">
         <v>197</v>
       </c>
     </row>
@@ -3495,7 +3511,7 @@
         <v>267</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C83" s="1" t="s">
         <v>12</v>
@@ -3507,13 +3523,13 @@
         <v>195</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="H83" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I83" s="1" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3547,7 +3563,7 @@
         <v>272</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="C85" s="1" t="s">
         <v>12</v>
@@ -3559,7 +3575,7 @@
         <v>195</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="H85" s="1" t="s">
         <v>16</v>
@@ -3654,25 +3670,25 @@
         <v>280</v>
       </c>
       <c r="C89" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E89" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="F89" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="D89" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E89" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="F89" s="1" t="s">
-        <v>253</v>
-      </c>
       <c r="G89" s="1" t="s">
-        <v>251</v>
+        <v>282</v>
       </c>
       <c r="H89" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I89" s="1" t="s">
-        <v>282</v>
+        <v>254</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3732,7 +3748,7 @@
         <v>288</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C92" s="1" t="s">
         <v>12</v>
@@ -3750,7 +3766,7 @@
         <v>16</v>
       </c>
       <c r="I92" s="1" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3831,32 +3847,32 @@
         <v>197</v>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A96" s="1" t="s">
+    <row r="96" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A96" s="3" t="s">
         <v>302</v>
       </c>
-      <c r="B96" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="C96" s="1" t="s">
+      <c r="B96" s="3" t="s">
         <v>251</v>
       </c>
-      <c r="D96" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E96" s="1" t="s">
+      <c r="C96" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="F96" s="1" t="s">
+      <c r="D96" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E96" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="F96" s="3" t="s">
         <v>253</v>
       </c>
-      <c r="G96" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="H96" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I96" s="1" t="s">
+      <c r="G96" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="H96" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I96" s="3" t="s">
         <v>254</v>
       </c>
     </row>
@@ -3905,6 +3921,9 @@
       <c r="F98" s="1" t="s">
         <v>307</v>
       </c>
+      <c r="G98" s="1" t="s">
+        <v>204</v>
+      </c>
       <c r="H98" s="1" t="s">
         <v>16</v>
       </c>
@@ -3946,19 +3965,19 @@
         <v>313</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="D100" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>195</v>
+        <v>314</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="G100" s="1" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="H100" s="1" t="s">
         <v>16</v>
@@ -3969,10 +3988,10 @@
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A101" s="1" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="C101" s="1" t="s">
         <v>12</v>
@@ -3984,10 +4003,10 @@
         <v>195</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="G101" s="1" t="s">
-        <v>281</v>
+        <v>204</v>
       </c>
       <c r="H101" s="1" t="s">
         <v>16</v>
@@ -3998,10 +4017,10 @@
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A102" s="1" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="C102" s="1" t="s">
         <v>12</v>
@@ -4013,10 +4032,10 @@
         <v>195</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="G102" s="1" t="s">
-        <v>281</v>
+        <v>204</v>
       </c>
       <c r="H102" s="1" t="s">
         <v>16</v>
@@ -4027,10 +4046,10 @@
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A103" s="1" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="C103" s="1" t="s">
         <v>12</v>
@@ -4042,10 +4061,10 @@
         <v>195</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="G103" s="1" t="s">
-        <v>281</v>
+        <v>204</v>
       </c>
       <c r="H103" s="1" t="s">
         <v>16</v>
@@ -4056,10 +4075,10 @@
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A104" s="1" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="C104" s="1" t="s">
         <v>12</v>
@@ -4071,10 +4090,10 @@
         <v>195</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="G104" s="1" t="s">
-        <v>281</v>
+        <v>204</v>
       </c>
       <c r="H104" s="1" t="s">
         <v>16</v>
@@ -4085,10 +4104,10 @@
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A105" s="1" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C105" s="1" t="s">
         <v>12</v>
@@ -4097,50 +4116,50 @@
         <v>12</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="F105" s="1" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="H105" s="1" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="I105" s="1" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A106" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D106" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E106" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="F106" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="H106" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="I106" s="1" t="s">
         <v>329</v>
-      </c>
-      <c r="B106" s="1" t="s">
-        <v>324</v>
-      </c>
-      <c r="C106" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D106" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E106" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="F106" s="1" t="s">
-        <v>326</v>
-      </c>
-      <c r="H106" s="1" t="s">
-        <v>327</v>
-      </c>
-      <c r="I106" s="1" t="s">
-        <v>328</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A107" s="1" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="C107" s="1" t="s">
         <v>12</v>
@@ -4149,24 +4168,24 @@
         <v>12</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="F107" s="1" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="H107" s="1" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="I107" s="1" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A108" s="1" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="C108" s="1" t="s">
         <v>12</v>
@@ -4175,24 +4194,24 @@
         <v>12</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="F108" s="1" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="H108" s="1" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="I108" s="1" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A109" s="1" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="C109" s="1" t="s">
         <v>12</v>
@@ -4210,41 +4229,41 @@
         <v>16</v>
       </c>
       <c r="I109" s="1" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A110" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D110" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E110" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F110" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H110" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I110" s="1" t="s">
         <v>344</v>
-      </c>
-      <c r="B110" s="1" t="s">
-        <v>342</v>
-      </c>
-      <c r="C110" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D110" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E110" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F110" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H110" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I110" s="1" t="s">
-        <v>343</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A111" s="1" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="C111" s="1" t="s">
         <v>12</v>
@@ -4262,15 +4281,15 @@
         <v>16</v>
       </c>
       <c r="I111" s="1" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A112" s="1" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="C112" s="1" t="s">
         <v>12</v>
@@ -4288,15 +4307,15 @@
         <v>16</v>
       </c>
       <c r="I112" s="1" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A113" s="1" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="C113" s="1" t="s">
         <v>12</v>
@@ -4314,15 +4333,15 @@
         <v>16</v>
       </c>
       <c r="I113" s="1" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A114" s="1" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="C114" s="1" t="s">
         <v>12</v>
@@ -4340,15 +4359,15 @@
         <v>16</v>
       </c>
       <c r="I114" s="1" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="1" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="C115" s="1" t="s">
         <v>12</v>
@@ -4366,41 +4385,41 @@
         <v>16</v>
       </c>
       <c r="I115" s="1" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D116" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E116" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F116" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H116" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I116" s="1" t="s">
         <v>352</v>
-      </c>
-      <c r="B116" s="1" t="s">
-        <v>350</v>
-      </c>
-      <c r="C116" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D116" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E116" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F116" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H116" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I116" s="1" t="s">
-        <v>351</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="1" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="C117" s="1" t="s">
         <v>12</v>
@@ -4418,15 +4437,15 @@
         <v>16</v>
       </c>
       <c r="I117" s="1" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="1" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="C118" s="1" t="s">
         <v>12</v>
@@ -4444,15 +4463,15 @@
         <v>16</v>
       </c>
       <c r="I118" s="1" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="1" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="C119" s="1" t="s">
         <v>12</v>
@@ -4470,15 +4489,15 @@
         <v>16</v>
       </c>
       <c r="I119" s="1" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="1" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="C120" s="1" t="s">
         <v>12</v>
@@ -4496,7 +4515,7 @@
         <v>16</v>
       </c>
       <c r="I120" s="1" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
LTC3: One last correction to charge controller BOM.
And I'm serious this time.
</commit_message>
<xml_diff>
--- a/ltc3/bom/charge_controller/LTC3_Charge_Controller.xlsx
+++ b/ltc3/bom/charge_controller/LTC3_Charge_Controller.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1011" uniqueCount="358">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1011" uniqueCount="357">
   <si>
     <t xml:space="preserve">Refs</t>
   </si>
@@ -887,9 +887,6 @@
   </si>
   <si>
     <t xml:space="preserve">R34</t>
-  </si>
-  <si>
-    <t xml:space="preserve">storm eye</t>
   </si>
   <si>
     <t xml:space="preserve">R35</t>
@@ -1227,8 +1224,8 @@
   </sheetPr>
   <dimension ref="A1:I120"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A72" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H98" activeCellId="0" sqref="H98"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A67" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F93" activeCellId="0" sqref="F93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -3760,7 +3757,7 @@
         <v>195</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>289</v>
+        <v>237</v>
       </c>
       <c r="H92" s="1" t="s">
         <v>16</v>
@@ -3771,22 +3768,22 @@
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A93" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="B93" s="1" t="s">
         <v>290</v>
       </c>
-      <c r="B93" s="1" t="s">
+      <c r="C93" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D93" s="1" t="s">
         <v>291</v>
-      </c>
-      <c r="C93" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D93" s="1" t="s">
-        <v>292</v>
       </c>
       <c r="E93" s="1" t="s">
         <v>195</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="H93" s="1" t="s">
         <v>16</v>
@@ -3797,22 +3794,22 @@
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A94" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="B94" s="1" t="s">
         <v>294</v>
       </c>
-      <c r="B94" s="1" t="s">
+      <c r="C94" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D94" s="1" t="s">
         <v>295</v>
-      </c>
-      <c r="C94" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D94" s="1" t="s">
-        <v>296</v>
       </c>
       <c r="E94" s="1" t="s">
         <v>195</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="H94" s="1" t="s">
         <v>16</v>
@@ -3823,22 +3820,22 @@
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A95" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="B95" s="1" t="s">
         <v>298</v>
       </c>
-      <c r="B95" s="1" t="s">
+      <c r="C95" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D95" s="1" t="s">
         <v>299</v>
-      </c>
-      <c r="C95" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D95" s="1" t="s">
-        <v>300</v>
       </c>
       <c r="E95" s="1" t="s">
         <v>195</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="H95" s="1" t="s">
         <v>16</v>
@@ -3849,7 +3846,7 @@
     </row>
     <row r="96" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A96" s="3" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B96" s="3" t="s">
         <v>251</v>
@@ -3878,7 +3875,7 @@
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A97" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B97" s="1" t="s">
         <v>256</v>
@@ -3904,22 +3901,22 @@
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A98" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="B98" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="B98" s="1" t="s">
+      <c r="C98" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D98" s="1" t="s">
         <v>305</v>
-      </c>
-      <c r="C98" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D98" s="1" t="s">
-        <v>306</v>
       </c>
       <c r="E98" s="1" t="s">
         <v>195</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="G98" s="1" t="s">
         <v>204</v>
@@ -3933,22 +3930,22 @@
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A99" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="B99" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="B99" s="1" t="s">
+      <c r="C99" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D99" s="1" t="s">
         <v>309</v>
-      </c>
-      <c r="C99" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D99" s="1" t="s">
-        <v>310</v>
       </c>
       <c r="E99" s="1" t="s">
         <v>195</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="H99" s="1" t="s">
         <v>16</v>
@@ -3959,10 +3956,10 @@
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A100" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="B100" s="1" t="s">
         <v>312</v>
-      </c>
-      <c r="B100" s="1" t="s">
-        <v>313</v>
       </c>
       <c r="C100" s="1" t="s">
         <v>252</v>
@@ -3971,10 +3968,10 @@
         <v>12</v>
       </c>
       <c r="E100" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="F100" s="1" t="s">
         <v>314</v>
-      </c>
-      <c r="F100" s="1" t="s">
-        <v>315</v>
       </c>
       <c r="G100" s="1" t="s">
         <v>252</v>
@@ -3988,10 +3985,10 @@
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A101" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="B101" s="1" t="s">
         <v>316</v>
-      </c>
-      <c r="B101" s="1" t="s">
-        <v>317</v>
       </c>
       <c r="C101" s="1" t="s">
         <v>12</v>
@@ -4003,7 +4000,7 @@
         <v>195</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="G101" s="1" t="s">
         <v>204</v>
@@ -4017,10 +4014,10 @@
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A102" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="B102" s="1" t="s">
         <v>319</v>
-      </c>
-      <c r="B102" s="1" t="s">
-        <v>320</v>
       </c>
       <c r="C102" s="1" t="s">
         <v>12</v>
@@ -4032,7 +4029,7 @@
         <v>195</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="G102" s="1" t="s">
         <v>204</v>
@@ -4046,10 +4043,10 @@
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A103" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C103" s="1" t="s">
         <v>12</v>
@@ -4061,7 +4058,7 @@
         <v>195</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="G103" s="1" t="s">
         <v>204</v>
@@ -4075,10 +4072,10 @@
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A104" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C104" s="1" t="s">
         <v>12</v>
@@ -4090,7 +4087,7 @@
         <v>195</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="G104" s="1" t="s">
         <v>204</v>
@@ -4104,418 +4101,418 @@
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A105" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="B105" s="1" t="s">
         <v>324</v>
       </c>
-      <c r="B105" s="1" t="s">
+      <c r="C105" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D105" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E105" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="C105" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D105" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E105" s="1" t="s">
+      <c r="F105" s="1" t="s">
         <v>326</v>
       </c>
-      <c r="F105" s="1" t="s">
+      <c r="H105" s="1" t="s">
         <v>327</v>
       </c>
-      <c r="H105" s="1" t="s">
+      <c r="I105" s="1" t="s">
         <v>328</v>
-      </c>
-      <c r="I105" s="1" t="s">
-        <v>329</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A106" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B106" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D106" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E106" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="C106" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D106" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E106" s="1" t="s">
+      <c r="F106" s="1" t="s">
         <v>326</v>
       </c>
-      <c r="F106" s="1" t="s">
+      <c r="H106" s="1" t="s">
         <v>327</v>
       </c>
-      <c r="H106" s="1" t="s">
+      <c r="I106" s="1" t="s">
         <v>328</v>
-      </c>
-      <c r="I106" s="1" t="s">
-        <v>329</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A107" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="B107" s="1" t="s">
         <v>331</v>
       </c>
-      <c r="B107" s="1" t="s">
+      <c r="C107" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D107" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E107" s="1" t="s">
         <v>332</v>
       </c>
-      <c r="C107" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D107" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E107" s="1" t="s">
+      <c r="F107" s="1" t="s">
         <v>333</v>
       </c>
-      <c r="F107" s="1" t="s">
+      <c r="H107" s="1" t="s">
         <v>334</v>
       </c>
-      <c r="H107" s="1" t="s">
+      <c r="I107" s="1" t="s">
         <v>335</v>
-      </c>
-      <c r="I107" s="1" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A108" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="B108" s="1" t="s">
         <v>337</v>
       </c>
-      <c r="B108" s="1" t="s">
+      <c r="C108" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D108" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E108" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="F108" s="1" t="s">
         <v>338</v>
       </c>
-      <c r="C108" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D108" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E108" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="F108" s="1" t="s">
+      <c r="H108" s="1" t="s">
         <v>339</v>
       </c>
-      <c r="H108" s="1" t="s">
+      <c r="I108" s="1" t="s">
         <v>340</v>
-      </c>
-      <c r="I108" s="1" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A109" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="B109" s="1" t="s">
         <v>342</v>
       </c>
-      <c r="B109" s="1" t="s">
+      <c r="C109" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D109" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E109" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F109" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H109" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I109" s="1" t="s">
         <v>343</v>
-      </c>
-      <c r="C109" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D109" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E109" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F109" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H109" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I109" s="1" t="s">
-        <v>344</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A110" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B110" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D110" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E110" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F110" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H110" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I110" s="1" t="s">
         <v>343</v>
-      </c>
-      <c r="C110" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D110" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E110" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F110" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H110" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I110" s="1" t="s">
-        <v>344</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A111" s="1" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B111" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D111" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E111" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F111" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H111" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I111" s="1" t="s">
         <v>343</v>
-      </c>
-      <c r="C111" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D111" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E111" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F111" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H111" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I111" s="1" t="s">
-        <v>344</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A112" s="1" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B112" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D112" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E112" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F112" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H112" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I112" s="1" t="s">
         <v>343</v>
-      </c>
-      <c r="C112" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D112" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E112" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F112" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H112" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I112" s="1" t="s">
-        <v>344</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A113" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B113" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D113" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E113" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F113" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H113" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I113" s="1" t="s">
         <v>343</v>
-      </c>
-      <c r="C113" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D113" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E113" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F113" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H113" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I113" s="1" t="s">
-        <v>344</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A114" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B114" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D114" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E114" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F114" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H114" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I114" s="1" t="s">
         <v>343</v>
-      </c>
-      <c r="C114" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D114" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E114" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F114" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H114" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I114" s="1" t="s">
-        <v>344</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="B115" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="B115" s="1" t="s">
+      <c r="C115" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D115" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E115" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F115" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H115" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I115" s="1" t="s">
         <v>351</v>
-      </c>
-      <c r="C115" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D115" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E115" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F115" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H115" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I115" s="1" t="s">
-        <v>352</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B116" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D116" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E116" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F116" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H116" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I116" s="1" t="s">
         <v>351</v>
-      </c>
-      <c r="C116" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D116" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E116" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F116" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H116" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I116" s="1" t="s">
-        <v>352</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B117" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D117" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E117" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F117" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H117" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I117" s="1" t="s">
         <v>351</v>
-      </c>
-      <c r="C117" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D117" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E117" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F117" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H117" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I117" s="1" t="s">
-        <v>352</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="1" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B118" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D118" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E118" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F118" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H118" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I118" s="1" t="s">
         <v>351</v>
-      </c>
-      <c r="C118" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D118" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E118" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F118" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H118" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I118" s="1" t="s">
-        <v>352</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B119" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D119" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E119" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F119" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H119" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I119" s="1" t="s">
         <v>343</v>
-      </c>
-      <c r="C119" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D119" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E119" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F119" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H119" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I119" s="1" t="s">
-        <v>344</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B120" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="C120" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D120" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E120" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F120" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H120" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I120" s="1" t="s">
         <v>343</v>
-      </c>
-      <c r="C120" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D120" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E120" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F120" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H120" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I120" s="1" t="s">
-        <v>344</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
LTC3: Corrected LTC2990 shunt resistor spec, etc.
I was only kidding about being finished.
</commit_message>
<xml_diff>
--- a/ltc3/bom/charge_controller/LTC3_Charge_Controller.xlsx
+++ b/ltc3/bom/charge_controller/LTC3_Charge_Controller.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1011" uniqueCount="357">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1011" uniqueCount="358">
   <si>
     <t xml:space="preserve">Refs</t>
   </si>
@@ -958,13 +958,16 @@
     <t xml:space="preserve">R42</t>
   </si>
   <si>
-    <t xml:space="preserve">100m</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Samsung</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RUW3216FR100CS</t>
+    <t xml:space="preserve">60m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1% 2W</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PE2512FKE7W0R06L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resistors_SMD:R_2512</t>
   </si>
   <si>
     <t xml:space="preserve">R43</t>
@@ -1188,7 +1191,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1198,6 +1201,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1224,8 +1231,8 @@
   </sheetPr>
   <dimension ref="A1:I120"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A67" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F93" activeCellId="0" sqref="F93"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A77" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E100" activeCellId="0" sqref="E100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -3958,37 +3965,37 @@
       <c r="A100" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="B100" s="1" t="s">
+      <c r="B100" s="4" t="s">
         <v>312</v>
       </c>
-      <c r="C100" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="D100" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E100" s="1" t="s">
+      <c r="C100" s="4" t="s">
         <v>313</v>
       </c>
-      <c r="F100" s="1" t="s">
+      <c r="D100" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E100" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="F100" s="4" t="s">
         <v>314</v>
       </c>
-      <c r="G100" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="H100" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I100" s="1" t="s">
-        <v>254</v>
+      <c r="G100" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="H100" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I100" s="4" t="s">
+        <v>315</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A101" s="1" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="C101" s="1" t="s">
         <v>12</v>
@@ -4000,7 +4007,7 @@
         <v>195</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="G101" s="1" t="s">
         <v>204</v>
@@ -4014,10 +4021,10 @@
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A102" s="1" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="C102" s="1" t="s">
         <v>12</v>
@@ -4029,7 +4036,7 @@
         <v>195</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="G102" s="1" t="s">
         <v>204</v>
@@ -4043,10 +4050,10 @@
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A103" s="1" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="C103" s="1" t="s">
         <v>12</v>
@@ -4058,7 +4065,7 @@
         <v>195</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="G103" s="1" t="s">
         <v>204</v>
@@ -4072,10 +4079,10 @@
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A104" s="1" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="C104" s="1" t="s">
         <v>12</v>
@@ -4087,7 +4094,7 @@
         <v>195</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="G104" s="1" t="s">
         <v>204</v>
@@ -4101,10 +4108,10 @@
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A105" s="1" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C105" s="1" t="s">
         <v>12</v>
@@ -4113,50 +4120,50 @@
         <v>12</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="F105" s="1" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="H105" s="1" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="I105" s="1" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A106" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D106" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E106" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="F106" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="H106" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="I106" s="1" t="s">
         <v>329</v>
-      </c>
-      <c r="B106" s="1" t="s">
-        <v>324</v>
-      </c>
-      <c r="C106" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D106" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E106" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="F106" s="1" t="s">
-        <v>326</v>
-      </c>
-      <c r="H106" s="1" t="s">
-        <v>327</v>
-      </c>
-      <c r="I106" s="1" t="s">
-        <v>328</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A107" s="1" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="C107" s="1" t="s">
         <v>12</v>
@@ -4165,24 +4172,24 @@
         <v>12</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="F107" s="1" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="H107" s="1" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="I107" s="1" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A108" s="1" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="C108" s="1" t="s">
         <v>12</v>
@@ -4191,24 +4198,24 @@
         <v>12</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="F108" s="1" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="H108" s="1" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="I108" s="1" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A109" s="1" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="C109" s="1" t="s">
         <v>12</v>
@@ -4226,41 +4233,41 @@
         <v>16</v>
       </c>
       <c r="I109" s="1" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A110" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D110" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E110" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F110" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H110" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I110" s="1" t="s">
         <v>344</v>
-      </c>
-      <c r="B110" s="1" t="s">
-        <v>342</v>
-      </c>
-      <c r="C110" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D110" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E110" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F110" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H110" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I110" s="1" t="s">
-        <v>343</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A111" s="1" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="C111" s="1" t="s">
         <v>12</v>
@@ -4278,15 +4285,15 @@
         <v>16</v>
       </c>
       <c r="I111" s="1" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A112" s="1" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="C112" s="1" t="s">
         <v>12</v>
@@ -4304,15 +4311,15 @@
         <v>16</v>
       </c>
       <c r="I112" s="1" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A113" s="1" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="C113" s="1" t="s">
         <v>12</v>
@@ -4330,15 +4337,15 @@
         <v>16</v>
       </c>
       <c r="I113" s="1" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A114" s="1" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="C114" s="1" t="s">
         <v>12</v>
@@ -4356,15 +4363,15 @@
         <v>16</v>
       </c>
       <c r="I114" s="1" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="1" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="C115" s="1" t="s">
         <v>12</v>
@@ -4382,41 +4389,41 @@
         <v>16</v>
       </c>
       <c r="I115" s="1" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D116" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E116" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F116" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H116" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I116" s="1" t="s">
         <v>352</v>
-      </c>
-      <c r="B116" s="1" t="s">
-        <v>350</v>
-      </c>
-      <c r="C116" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D116" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E116" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F116" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H116" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I116" s="1" t="s">
-        <v>351</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="1" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="C117" s="1" t="s">
         <v>12</v>
@@ -4434,15 +4441,15 @@
         <v>16</v>
       </c>
       <c r="I117" s="1" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="1" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="C118" s="1" t="s">
         <v>12</v>
@@ -4460,15 +4467,15 @@
         <v>16</v>
       </c>
       <c r="I118" s="1" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="1" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="C119" s="1" t="s">
         <v>12</v>
@@ -4486,15 +4493,15 @@
         <v>16</v>
       </c>
       <c r="I119" s="1" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="1" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="C120" s="1" t="s">
         <v>12</v>
@@ -4512,7 +4519,7 @@
         <v>16</v>
       </c>
       <c r="I120" s="1" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
LTC3: Minor modification to Charge Controller DC input connectors.
Combined P1 (PV_IN) and P2 (LAB_IN) connectors into a single 2x2
(4-pos) MicroFit connector (DC_IN).
</commit_message>
<xml_diff>
--- a/ltc3/bom/charge_controller/LTC3_Charge_Controller.xlsx
+++ b/ltc3/bom/charge_controller/LTC3_Charge_Controller.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1011" uniqueCount="358">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1008" uniqueCount="361">
   <si>
     <t xml:space="preserve">Refs</t>
   </si>
@@ -463,55 +463,64 @@
     <t xml:space="preserve">MicroFit header</t>
   </si>
   <si>
-    <t xml:space="preserve">PV_IN</t>
+    <t xml:space="preserve">DC_IN</t>
   </si>
   <si>
     <t xml:space="preserve">Molex</t>
   </si>
   <si>
+    <t xml:space="preserve">43045-0428</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4-pos vertical header</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/psas/launch-tower/blob/master/ltc3/doc/datasheets/connectors/Molex-43045-Micro_Fit_3_dual_row_vertical_through_hole_header.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Connectors_Molex:Molex_Microfit3_Header_02x02_Straight_43045-0428</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XH header</t>
+  </si>
+  <si>
+    <t xml:space="preserve">to thermistor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B2B-XH-A(LF)(SN)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-pos vertical header</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/psas/launch-tower/blob/master/ltc3/doc/datasheets/connectors/JST-XH-2.5mm_pitch_Disconnectable_Crimp_style_connectors.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Connectors_JST:JST_XH_B02B-XH-A_02x2.50mm_Straight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">to cell protection</t>
+  </si>
+  <si>
     <t xml:space="preserve">43045-0228</t>
   </si>
   <si>
-    <t xml:space="preserve">https://github.com/psas/launch-tower/blob/master/ltc3/doc/datasheets/connectors/Molex-43045-Micro_Fit_3_dual_row_vertical_through_hole_header.pdf</t>
-  </si>
-  <si>
     <t xml:space="preserve">Connectors_Molex:Molex_Microfit3_Header_02x01_Straight_43045-0228</t>
   </si>
   <si>
-    <t xml:space="preserve">P2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LAB_IN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Connectors_Molex:Molex_Microfit3_Header_02x02_Straight_43045-0428</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">XH header</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JST</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B2B-XH-A(LF)(SN)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://github.com/psas/launch-tower/blob/master/ltc3/doc/datasheets/connectors/JST-XH-2.5mm_pitch_Disconnectable_Crimp_style_connectors.pdf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Connectors_JST:JST_XH_B02B-XH-A_02x2.50mm_Straight</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P4</t>
-  </si>
-  <si>
     <t xml:space="preserve">P5</t>
   </si>
   <si>
-    <t xml:space="preserve">To LTC</t>
+    <t xml:space="preserve">to LTC</t>
   </si>
   <si>
     <t xml:space="preserve">Connectors_JST:JST_EH_B02B-XH-A_02x2.50mm_Straight</t>
@@ -1191,7 +1200,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1201,14 +1210,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1229,10 +1230,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I120"/>
+  <dimension ref="A1:I119"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A23" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B51" activeCellId="0" sqref="B51"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D51" activeCellId="0" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1241,11 +1242,11 @@
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.9271255060729"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="1" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="16.497975708502"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="12.748987854251"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="22.8178137651822"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="22.1740890688259"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="20.8866396761134"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="65.7692307692308"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="12.8542510121458"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="22.9230769230769"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="22.3886639676113"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="20.995951417004"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="66.3076923076923"/>
     <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -2552,146 +2553,161 @@
       <c r="F46" s="1" t="s">
         <v>149</v>
       </c>
+      <c r="G46" s="1" t="s">
+        <v>150</v>
+      </c>
       <c r="H46" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>149</v>
+        <v>157</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>158</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>150</v>
+        <v>159</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>12</v>
+        <v>162</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="F48" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="G48" s="1" t="s">
         <v>158</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>12</v>
+        <v>166</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>149</v>
+        <v>157</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>158</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>150</v>
+        <v>159</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>154</v>
+        <v>167</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="B50" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="E50" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="C50" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>157</v>
-      </c>
       <c r="F50" s="1" t="s">
-        <v>158</v>
+        <v>169</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>150</v>
       </c>
       <c r="H50" s="1" t="s">
         <v>159</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>156</v>
+        <v>172</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>163</v>
+        <v>12</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>157</v>
+        <v>173</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>166</v>
+        <v>174</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>159</v>
+        <v>175</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>167</v>
+        <v>176</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>168</v>
+        <v>177</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>169</v>
+        <v>178</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>12</v>
@@ -2700,24 +2716,24 @@
         <v>12</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>172</v>
+        <v>180</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>173</v>
+        <v>181</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
-        <v>174</v>
+        <v>182</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>12</v>
@@ -2726,76 +2742,76 @@
         <v>12</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E54" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="B54" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E54" s="1" t="s">
-        <v>176</v>
-      </c>
       <c r="F54" s="1" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="H55" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="B55" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E55" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="F55" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="H55" s="1" t="s">
-        <v>177</v>
-      </c>
       <c r="I55" s="1" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>175</v>
+        <v>186</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>12</v>
@@ -2804,24 +2820,24 @@
         <v>12</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>176</v>
+        <v>130</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>175</v>
+        <v>187</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>177</v>
+        <v>188</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>178</v>
+        <v>189</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>183</v>
+        <v>191</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>12</v>
@@ -2830,102 +2846,105 @@
         <v>12</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>130</v>
+        <v>192</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>184</v>
+        <v>193</v>
       </c>
       <c r="H57" s="1" t="s">
-        <v>185</v>
+        <v>194</v>
       </c>
       <c r="I57" s="1" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>188</v>
+        <v>196</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>12</v>
+        <v>197</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>189</v>
+        <v>198</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>191</v>
+        <v>16</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>186</v>
+        <v>200</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>193</v>
+        <v>202</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>196</v>
+        <v>203</v>
       </c>
       <c r="H59" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I59" s="1" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E60" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="B60" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E60" s="1" t="s">
-        <v>195</v>
-      </c>
       <c r="F60" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="H60" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I60" s="1" t="s">
         <v>200</v>
-      </c>
-      <c r="H60" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I60" s="1" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
-        <v>201</v>
+        <v>208</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>12</v>
@@ -2934,27 +2953,27 @@
         <v>12</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="H61" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I61" s="1" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>202</v>
+        <v>210</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>12</v>
@@ -2963,27 +2982,27 @@
         <v>12</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>203</v>
+        <v>211</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>204</v>
+        <v>212</v>
       </c>
       <c r="H62" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I62" s="1" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
-        <v>206</v>
+        <v>213</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>12</v>
@@ -2992,27 +3011,27 @@
         <v>12</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="H63" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I63" s="1" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>207</v>
+        <v>215</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>12</v>
@@ -3021,27 +3040,24 @@
         <v>12</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="G64" s="1" t="s">
-        <v>209</v>
+        <v>216</v>
       </c>
       <c r="H64" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I64" s="1" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
-        <v>211</v>
+        <v>217</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>212</v>
+        <v>218</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>12</v>
@@ -3050,102 +3066,102 @@
         <v>12</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>213</v>
+        <v>219</v>
       </c>
       <c r="H65" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I65" s="1" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
-        <v>214</v>
+        <v>220</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>215</v>
+        <v>221</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>12</v>
+        <v>197</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="H66" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I66" s="1" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
-        <v>217</v>
+        <v>223</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>195</v>
+        <v>225</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>219</v>
+        <v>226</v>
       </c>
       <c r="H67" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I67" s="1" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="68" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A68" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="B68" s="3" t="s">
-        <v>221</v>
-      </c>
-      <c r="C68" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="D68" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E68" s="3" t="s">
-        <v>222</v>
-      </c>
-      <c r="F68" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="H68" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I68" s="3" t="s">
-        <v>197</v>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A68" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="H68" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I68" s="1" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>12</v>
@@ -3154,24 +3170,24 @@
         <v>12</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
       <c r="H69" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I69" s="1" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>12</v>
@@ -3180,24 +3196,24 @@
         <v>12</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>229</v>
+        <v>235</v>
       </c>
       <c r="H70" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I70" s="1" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>12</v>
@@ -3206,24 +3222,24 @@
         <v>12</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>232</v>
+        <v>238</v>
       </c>
       <c r="H71" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I71" s="1" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
-        <v>233</v>
+        <v>239</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>234</v>
+        <v>210</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>12</v>
@@ -3232,24 +3248,24 @@
         <v>12</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="H72" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I72" s="1" t="s">
-        <v>197</v>
+        <v>241</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
-        <v>236</v>
+        <v>242</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>207</v>
+        <v>243</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>12</v>
@@ -3258,24 +3274,24 @@
         <v>12</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>195</v>
+        <v>244</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>237</v>
+        <v>245</v>
       </c>
       <c r="H73" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I73" s="1" t="s">
-        <v>238</v>
+        <v>200</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="s">
-        <v>239</v>
+        <v>246</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>240</v>
+        <v>247</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>12</v>
@@ -3284,24 +3300,24 @@
         <v>12</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>241</v>
+        <v>198</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>242</v>
+        <v>248</v>
       </c>
       <c r="H74" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I74" s="1" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="13.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="s">
-        <v>243</v>
+        <v>249</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>244</v>
+        <v>250</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>12</v>
@@ -3310,24 +3326,24 @@
         <v>12</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>245</v>
+        <v>251</v>
       </c>
       <c r="H75" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I75" s="1" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="76" customFormat="false" ht="13.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>247</v>
+        <v>205</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>12</v>
@@ -3336,264 +3352,264 @@
         <v>12</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>248</v>
+        <v>206</v>
+      </c>
+      <c r="G76" s="1" t="s">
+        <v>207</v>
       </c>
       <c r="H76" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I76" s="1" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>202</v>
+        <v>254</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>12</v>
+        <v>255</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>195</v>
+        <v>244</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>203</v>
+        <v>256</v>
       </c>
       <c r="G77" s="1" t="s">
-        <v>204</v>
+        <v>255</v>
       </c>
       <c r="H77" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I77" s="1" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="78" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A78" s="3" t="s">
-        <v>250</v>
-      </c>
-      <c r="B78" s="3" t="s">
-        <v>251</v>
-      </c>
-      <c r="C78" s="3" t="s">
-        <v>252</v>
-      </c>
-      <c r="D78" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E78" s="3" t="s">
-        <v>241</v>
-      </c>
-      <c r="F78" s="3" t="s">
-        <v>253</v>
-      </c>
-      <c r="G78" s="3" t="s">
-        <v>252</v>
-      </c>
-      <c r="H78" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I78" s="3" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="79" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A79" s="3" t="s">
-        <v>255</v>
-      </c>
-      <c r="B79" s="3" t="s">
-        <v>256</v>
-      </c>
-      <c r="C79" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D79" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E79" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="F79" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="H79" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I79" s="3" t="s">
-        <v>197</v>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A78" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="F78" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="H78" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I78" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A79" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="F79" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="H79" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I79" s="1" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="s">
-        <v>258</v>
+        <v>264</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>259</v>
+        <v>265</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>12</v>
+        <v>266</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>260</v>
+        <v>267</v>
       </c>
       <c r="H80" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I80" s="1" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A81" s="1" t="s">
-        <v>261</v>
+        <v>268</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>263</v>
+        <v>269</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="H81" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I81" s="1" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A82" s="1" t="s">
-        <v>265</v>
+        <v>270</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>262</v>
+        <v>210</v>
       </c>
       <c r="C82" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>266</v>
+        <v>12</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>264</v>
+        <v>240</v>
       </c>
       <c r="H82" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I82" s="1" t="s">
-        <v>197</v>
+        <v>241</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A83" s="1" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>207</v>
+        <v>272</v>
       </c>
       <c r="C83" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>12</v>
+        <v>273</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>237</v>
+        <v>274</v>
       </c>
       <c r="H83" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I83" s="1" t="s">
-        <v>238</v>
+        <v>200</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A84" s="1" t="s">
-        <v>268</v>
+        <v>275</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>269</v>
+        <v>231</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>270</v>
+        <v>276</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>271</v>
+        <v>232</v>
       </c>
       <c r="H84" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I84" s="1" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A85" s="1" t="s">
-        <v>272</v>
+        <v>277</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>228</v>
+        <v>259</v>
       </c>
       <c r="C85" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>273</v>
+        <v>12</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>229</v>
+        <v>260</v>
       </c>
       <c r="H85" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I85" s="1" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A86" s="1" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>12</v>
@@ -3602,24 +3618,24 @@
         <v>12</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="H86" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I86" s="1" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A87" s="1" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>256</v>
+        <v>280</v>
       </c>
       <c r="C87" s="1" t="s">
         <v>12</v>
@@ -3628,374 +3644,377 @@
         <v>12</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>257</v>
+        <v>281</v>
       </c>
       <c r="H87" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I87" s="1" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A88" s="1" t="s">
-        <v>276</v>
+        <v>282</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>277</v>
+        <v>283</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>12</v>
+        <v>207</v>
       </c>
       <c r="D88" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>195</v>
+        <v>244</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>278</v>
+        <v>284</v>
+      </c>
+      <c r="G88" s="1" t="s">
+        <v>285</v>
       </c>
       <c r="H88" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I88" s="1" t="s">
-        <v>197</v>
+        <v>257</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A89" s="1" t="s">
-        <v>279</v>
+        <v>286</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>280</v>
+        <v>287</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>204</v>
+        <v>12</v>
       </c>
       <c r="D89" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>241</v>
+        <v>198</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>281</v>
-      </c>
-      <c r="G89" s="1" t="s">
-        <v>282</v>
+        <v>288</v>
       </c>
       <c r="H89" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I89" s="1" t="s">
-        <v>254</v>
+        <v>200</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A90" s="1" t="s">
-        <v>283</v>
+        <v>289</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="C90" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>12</v>
+        <v>290</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="H90" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I90" s="1" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A91" s="1" t="s">
-        <v>286</v>
+        <v>291</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>284</v>
+        <v>210</v>
       </c>
       <c r="C91" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>287</v>
+        <v>12</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>285</v>
+        <v>240</v>
       </c>
       <c r="H91" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I91" s="1" t="s">
-        <v>197</v>
+        <v>241</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A92" s="1" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>207</v>
+        <v>293</v>
       </c>
       <c r="C92" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>12</v>
+        <v>294</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>237</v>
+        <v>295</v>
       </c>
       <c r="H92" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I92" s="1" t="s">
-        <v>238</v>
+        <v>200</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A93" s="1" t="s">
-        <v>289</v>
+        <v>296</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>290</v>
+        <v>297</v>
       </c>
       <c r="C93" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>291</v>
+        <v>298</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>292</v>
+        <v>299</v>
       </c>
       <c r="H93" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I93" s="1" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A94" s="1" t="s">
-        <v>293</v>
+        <v>300</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>294</v>
+        <v>301</v>
       </c>
       <c r="C94" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>295</v>
+        <v>302</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>296</v>
+        <v>303</v>
       </c>
       <c r="H94" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I94" s="1" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A95" s="1" t="s">
-        <v>297</v>
+        <v>304</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>298</v>
+        <v>254</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>12</v>
+        <v>255</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>299</v>
+        <v>12</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>195</v>
+        <v>244</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>300</v>
+        <v>256</v>
+      </c>
+      <c r="G95" s="1" t="s">
+        <v>255</v>
       </c>
       <c r="H95" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I95" s="1" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="96" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A96" s="3" t="s">
-        <v>301</v>
-      </c>
-      <c r="B96" s="3" t="s">
-        <v>251</v>
-      </c>
-      <c r="C96" s="3" t="s">
-        <v>252</v>
-      </c>
-      <c r="D96" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E96" s="3" t="s">
-        <v>241</v>
-      </c>
-      <c r="F96" s="3" t="s">
-        <v>253</v>
-      </c>
-      <c r="G96" s="3" t="s">
-        <v>252</v>
-      </c>
-      <c r="H96" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I96" s="3" t="s">
-        <v>254</v>
+        <v>257</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A96" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E96" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="F96" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="H96" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I96" s="1" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A97" s="1" t="s">
-        <v>302</v>
+        <v>306</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>256</v>
+        <v>307</v>
       </c>
       <c r="C97" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>12</v>
+        <v>308</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>257</v>
+        <v>309</v>
+      </c>
+      <c r="G97" s="1" t="s">
+        <v>207</v>
       </c>
       <c r="H97" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I97" s="1" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A98" s="1" t="s">
-        <v>303</v>
+        <v>310</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>304</v>
+        <v>311</v>
       </c>
       <c r="C98" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>305</v>
+        <v>312</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="G98" s="1" t="s">
-        <v>204</v>
+        <v>313</v>
       </c>
       <c r="H98" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I98" s="1" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A99" s="1" t="s">
-        <v>307</v>
+        <v>314</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>308</v>
+        <v>315</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>12</v>
+        <v>316</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>309</v>
+        <v>12</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>310</v>
+        <v>317</v>
+      </c>
+      <c r="G99" s="1" t="s">
+        <v>316</v>
       </c>
       <c r="H99" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I99" s="1" t="s">
-        <v>197</v>
+        <v>318</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A100" s="1" t="s">
-        <v>311</v>
-      </c>
-      <c r="B100" s="4" t="s">
-        <v>312</v>
-      </c>
-      <c r="C100" s="4" t="s">
-        <v>313</v>
-      </c>
-      <c r="D100" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E100" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="F100" s="4" t="s">
-        <v>314</v>
-      </c>
-      <c r="G100" s="4" t="s">
-        <v>313</v>
-      </c>
-      <c r="H100" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="I100" s="4" t="s">
-        <v>315</v>
+        <v>319</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D100" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E100" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="F100" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="G100" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="H100" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I100" s="1" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A101" s="1" t="s">
-        <v>316</v>
+        <v>322</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>317</v>
+        <v>323</v>
       </c>
       <c r="C101" s="1" t="s">
         <v>12</v>
@@ -4004,24 +4023,24 @@
         <v>12</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>318</v>
+        <v>324</v>
       </c>
       <c r="G101" s="1" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="H101" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I101" s="1" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A102" s="1" t="s">
-        <v>319</v>
+        <v>325</v>
       </c>
       <c r="B102" s="1" t="s">
         <v>320</v>
@@ -4033,27 +4052,27 @@
         <v>12</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="F102" s="1" t="s">
         <v>321</v>
       </c>
       <c r="G102" s="1" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="H102" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I102" s="1" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A103" s="1" t="s">
-        <v>322</v>
+        <v>326</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>317</v>
+        <v>323</v>
       </c>
       <c r="C103" s="1" t="s">
         <v>12</v>
@@ -4062,27 +4081,27 @@
         <v>12</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>318</v>
+        <v>324</v>
       </c>
       <c r="G103" s="1" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="H103" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I103" s="1" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A104" s="1" t="s">
-        <v>323</v>
+        <v>327</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>320</v>
+        <v>328</v>
       </c>
       <c r="C104" s="1" t="s">
         <v>12</v>
@@ -4091,27 +4110,24 @@
         <v>12</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>195</v>
+        <v>329</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>321</v>
-      </c>
-      <c r="G104" s="1" t="s">
-        <v>204</v>
+        <v>330</v>
       </c>
       <c r="H104" s="1" t="s">
-        <v>16</v>
+        <v>331</v>
       </c>
       <c r="I104" s="1" t="s">
-        <v>197</v>
+        <v>332</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A105" s="1" t="s">
-        <v>324</v>
+        <v>333</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="C105" s="1" t="s">
         <v>12</v>
@@ -4120,24 +4136,24 @@
         <v>12</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>326</v>
+        <v>329</v>
       </c>
       <c r="F105" s="1" t="s">
-        <v>327</v>
+        <v>330</v>
       </c>
       <c r="H105" s="1" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
       <c r="I105" s="1" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A106" s="1" t="s">
-        <v>330</v>
+        <v>334</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>325</v>
+        <v>335</v>
       </c>
       <c r="C106" s="1" t="s">
         <v>12</v>
@@ -4146,24 +4162,24 @@
         <v>12</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>326</v>
+        <v>336</v>
       </c>
       <c r="F106" s="1" t="s">
-        <v>327</v>
+        <v>337</v>
       </c>
       <c r="H106" s="1" t="s">
-        <v>328</v>
+        <v>338</v>
       </c>
       <c r="I106" s="1" t="s">
-        <v>329</v>
+        <v>339</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A107" s="1" t="s">
-        <v>331</v>
+        <v>340</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>332</v>
+        <v>341</v>
       </c>
       <c r="C107" s="1" t="s">
         <v>12</v>
@@ -4172,24 +4188,24 @@
         <v>12</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>333</v>
+        <v>336</v>
       </c>
       <c r="F107" s="1" t="s">
-        <v>334</v>
+        <v>342</v>
       </c>
       <c r="H107" s="1" t="s">
-        <v>335</v>
+        <v>343</v>
       </c>
       <c r="I107" s="1" t="s">
-        <v>336</v>
+        <v>344</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A108" s="1" t="s">
-        <v>337</v>
+        <v>345</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>338</v>
+        <v>346</v>
       </c>
       <c r="C108" s="1" t="s">
         <v>12</v>
@@ -4198,24 +4214,24 @@
         <v>12</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>333</v>
+        <v>12</v>
       </c>
       <c r="F108" s="1" t="s">
-        <v>339</v>
+        <v>12</v>
       </c>
       <c r="H108" s="1" t="s">
-        <v>340</v>
+        <v>16</v>
       </c>
       <c r="I108" s="1" t="s">
-        <v>341</v>
+        <v>347</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A109" s="1" t="s">
-        <v>342</v>
+        <v>348</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="C109" s="1" t="s">
         <v>12</v>
@@ -4233,15 +4249,15 @@
         <v>16</v>
       </c>
       <c r="I109" s="1" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A110" s="1" t="s">
-        <v>345</v>
+        <v>349</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="C110" s="1" t="s">
         <v>12</v>
@@ -4259,16 +4275,16 @@
         <v>16</v>
       </c>
       <c r="I110" s="1" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A111" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="B111" s="1" t="s">
         <v>346</v>
       </c>
-      <c r="B111" s="1" t="s">
-        <v>343</v>
-      </c>
       <c r="C111" s="1" t="s">
         <v>12</v>
       </c>
@@ -4285,41 +4301,41 @@
         <v>16</v>
       </c>
       <c r="I111" s="1" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A112" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D112" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E112" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F112" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H112" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I112" s="1" t="s">
         <v>347</v>
-      </c>
-      <c r="B112" s="1" t="s">
-        <v>343</v>
-      </c>
-      <c r="C112" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D112" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E112" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F112" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H112" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I112" s="1" t="s">
-        <v>344</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A113" s="1" t="s">
-        <v>348</v>
+        <v>352</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="C113" s="1" t="s">
         <v>12</v>
@@ -4337,15 +4353,15 @@
         <v>16</v>
       </c>
       <c r="I113" s="1" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="1" t="s">
-        <v>349</v>
+        <v>353</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>343</v>
+        <v>354</v>
       </c>
       <c r="C114" s="1" t="s">
         <v>12</v>
@@ -4363,15 +4379,15 @@
         <v>16</v>
       </c>
       <c r="I114" s="1" t="s">
-        <v>344</v>
+        <v>355</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="1" t="s">
-        <v>350</v>
+        <v>356</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="C115" s="1" t="s">
         <v>12</v>
@@ -4389,15 +4405,15 @@
         <v>16</v>
       </c>
       <c r="I115" s="1" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="1" t="s">
-        <v>353</v>
+        <v>357</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="C116" s="1" t="s">
         <v>12</v>
@@ -4415,16 +4431,16 @@
         <v>16</v>
       </c>
       <c r="I116" s="1" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="B117" s="1" t="s">
         <v>354</v>
       </c>
-      <c r="B117" s="1" t="s">
-        <v>351</v>
-      </c>
       <c r="C117" s="1" t="s">
         <v>12</v>
       </c>
@@ -4441,15 +4457,15 @@
         <v>16</v>
       </c>
       <c r="I117" s="1" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="1" t="s">
-        <v>355</v>
+        <v>359</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="C118" s="1" t="s">
         <v>12</v>
@@ -4467,15 +4483,15 @@
         <v>16</v>
       </c>
       <c r="I118" s="1" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="1" t="s">
-        <v>356</v>
+        <v>360</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="C119" s="1" t="s">
         <v>12</v>
@@ -4493,33 +4509,7 @@
         <v>16</v>
       </c>
       <c r="I119" s="1" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A120" s="1" t="s">
-        <v>357</v>
-      </c>
-      <c r="B120" s="1" t="s">
-        <v>343</v>
-      </c>
-      <c r="C120" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D120" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E120" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F120" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H120" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I120" s="1" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
LTC3: Minor changes to Charge Controller BOM.
Nothing that impacts PCB layout.
</commit_message>
<xml_diff>
--- a/ltc3/bom/charge_controller/LTC3_Charge_Controller.xlsx
+++ b/ltc3/bom/charge_controller/LTC3_Charge_Controller.xlsx
@@ -472,7 +472,7 @@
     <t xml:space="preserve">43045-0428</t>
   </si>
   <si>
-    <t xml:space="preserve">4-pos vertical header</t>
+    <t xml:space="preserve">4 pos vertical header</t>
   </si>
   <si>
     <t xml:space="preserve">https://github.com/psas/launch-tower/blob/master/ltc3/doc/datasheets/connectors/Molex-43045-Micro_Fit_3_dual_row_vertical_through_hole_header.pdf</t>
@@ -496,7 +496,7 @@
     <t xml:space="preserve">B2B-XH-A(LF)(SN)</t>
   </si>
   <si>
-    <t xml:space="preserve">2-pos vertical header</t>
+    <t xml:space="preserve">2 pos vertical header</t>
   </si>
   <si>
     <t xml:space="preserve">https://github.com/psas/launch-tower/blob/master/ltc3/doc/datasheets/connectors/JST-XH-2.5mm_pitch_Disconnectable_Crimp_style_connectors.pdf</t>
@@ -1232,22 +1232,22 @@
   </sheetPr>
   <dimension ref="A1:I119"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D51" activeCellId="0" sqref="D51"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A27" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G51" activeCellId="0" sqref="G51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="5.46153846153846"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.9271255060729"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="16.497975708502"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="12.8542510121458"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="22.9230769230769"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="22.3886639676113"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="20.995951417004"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="66.3076923076923"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="5.26530612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="22.5459183673469"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="22.1377551020408"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="47.9489795918367"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="65.469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="20.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
LTC3: Updated BOM info to reflect recent Charge Controller changes.
1. DC in and out connectors had their pin count doubled.
2. Opto-isolator added to LT8490 STATUS UART pin.
3. Zero-ohm resistors added to a few LT8490 option pins.
</commit_message>
<xml_diff>
--- a/ltc3/bom/charge_controller/LTC3_Charge_Controller.xlsx
+++ b/ltc3/bom/charge_controller/LTC3_Charge_Controller.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1008" uniqueCount="361">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1115" uniqueCount="374">
   <si>
     <t xml:space="preserve">Refs</t>
   </si>
@@ -469,15 +469,30 @@
     <t xml:space="preserve">Molex</t>
   </si>
   <si>
+    <t xml:space="preserve">43045-0828</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 pos vertical header</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/psas/launch-tower/blob/master/ltc3/doc/datasheets/connectors/Molex-43045-Micro_Fit_3_dual_row_vertical_through_hole_header.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Connectors_Molex:Molex_Microfit3_Header_02x04_Straight_43045-0828</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DC_OUT</t>
+  </si>
+  <si>
     <t xml:space="preserve">43045-0428</t>
   </si>
   <si>
     <t xml:space="preserve">4 pos vertical header</t>
   </si>
   <si>
-    <t xml:space="preserve">https://github.com/psas/launch-tower/blob/master/ltc3/doc/datasheets/connectors/Molex-43045-Micro_Fit_3_dual_row_vertical_through_hole_header.pdf</t>
-  </si>
-  <si>
     <t xml:space="preserve">Connectors_Molex:Molex_Microfit3_Header_02x02_Straight_43045-0428</t>
   </si>
   <si>
@@ -1003,6 +1018,18 @@
     <t xml:space="preserve">R46</t>
   </si>
   <si>
+    <t xml:space="preserve">R47</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TBD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R48</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R49</t>
+  </si>
+  <si>
     <t xml:space="preserve">U1</t>
   </si>
   <si>
@@ -1055,6 +1082,18 @@
   </si>
   <si>
     <t xml:space="preserve">LTC3:MSOP-10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4N25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">opto-isolator, 1-ch, 2500Vrms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Housings_DIP:DIP-6_W7.62mm</t>
   </si>
   <si>
     <t xml:space="preserve">W1</t>
@@ -1112,7 +1151,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1149,6 +1188,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1200,7 +1245,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1210,6 +1255,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1230,24 +1283,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I119"/>
+  <dimension ref="A1:I124"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A27" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G51" activeCellId="0" sqref="G51"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G46" activeCellId="0" sqref="G46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="5.26530612244898"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="22.5459183673469"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="22.1377551020408"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="47.9489795918367"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="65.469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="5.12755102040816"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="22.2755102040816"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="23.1530612244898"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="47.3826530612245"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="64.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="20.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2371,6 +2424,9 @@
       <c r="F39" s="1" t="s">
         <v>111</v>
       </c>
+      <c r="G39" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="H39" s="1" t="s">
         <v>112</v>
       </c>
@@ -2397,6 +2453,9 @@
       <c r="F40" s="1" t="s">
         <v>111</v>
       </c>
+      <c r="G40" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="H40" s="1" t="s">
         <v>112</v>
       </c>
@@ -2423,6 +2482,9 @@
       <c r="F41" s="1" t="s">
         <v>119</v>
       </c>
+      <c r="G41" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="H41" s="1" t="s">
         <v>120</v>
       </c>
@@ -2449,6 +2511,9 @@
       <c r="F42" s="1" t="s">
         <v>125</v>
       </c>
+      <c r="G42" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="H42" s="1" t="s">
         <v>126</v>
       </c>
@@ -2475,6 +2540,9 @@
       <c r="F43" s="1" t="s">
         <v>131</v>
       </c>
+      <c r="G43" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="H43" s="1" t="s">
         <v>132</v>
       </c>
@@ -2501,6 +2569,9 @@
       <c r="F44" s="1" t="s">
         <v>136</v>
       </c>
+      <c r="G44" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="H44" s="1" t="s">
         <v>137</v>
       </c>
@@ -2527,6 +2598,9 @@
       <c r="F45" s="1" t="s">
         <v>142</v>
       </c>
+      <c r="G45" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="H45" s="1" t="s">
         <v>143</v>
       </c>
@@ -2556,7 +2630,7 @@
       <c r="G46" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="H46" s="1" t="s">
+      <c r="H46" s="3" t="s">
         <v>151</v>
       </c>
       <c r="I46" s="1" t="s">
@@ -2568,158 +2642,164 @@
         <v>153</v>
       </c>
       <c r="B47" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D47" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="C47" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D47" s="1" t="s">
+      <c r="E47" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="F47" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="E47" s="1" t="s">
+      <c r="G47" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="F47" s="1" t="s">
+      <c r="H47" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="I47" s="3" t="s">
         <v>157</v>
-      </c>
-      <c r="G47" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="H47" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="I47" s="1" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="E48" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="B48" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D48" s="1" t="s">
+      <c r="F48" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="E48" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="F48" s="1" t="s">
+      <c r="G48" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="G48" s="1" t="s">
-        <v>158</v>
-      </c>
       <c r="H48" s="1" t="s">
-        <v>151</v>
+        <v>164</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>157</v>
+        <v>168</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>154</v>
+        <v>159</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>150</v>
+        <v>163</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="D51" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="B51" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="E51" s="1" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
       <c r="F51" s="1" t="s">
         <v>174</v>
       </c>
+      <c r="G51" s="1" t="s">
+        <v>156</v>
+      </c>
       <c r="H51" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="I51" s="1" t="s">
         <v>175</v>
-      </c>
-      <c r="I51" s="1" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B52" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="C52" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E52" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="C52" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E52" s="1" t="s">
+      <c r="F52" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="F52" s="1" t="s">
-        <v>178</v>
+      <c r="G52" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="H52" s="1" t="s">
         <v>180</v>
@@ -2733,7 +2813,7 @@
         <v>182</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>12</v>
@@ -2742,25 +2822,28 @@
         <v>12</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>178</v>
+        <v>183</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="B54" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="B54" s="1" t="s">
-        <v>178</v>
-      </c>
       <c r="C54" s="1" t="s">
         <v>12</v>
       </c>
@@ -2768,68 +2851,77 @@
         <v>12</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>178</v>
+        <v>183</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E55" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="B55" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E55" s="1" t="s">
-        <v>179</v>
-      </c>
       <c r="F55" s="1" t="s">
-        <v>178</v>
+        <v>183</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H56" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="B56" s="1" t="s">
+      <c r="I56" s="1" t="s">
         <v>186</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E56" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="F56" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="H56" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="I56" s="1" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2846,16 +2938,19 @@
         <v>12</v>
       </c>
       <c r="E57" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="F57" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="F57" s="1" t="s">
+      <c r="G57" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H57" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="H57" s="1" t="s">
+      <c r="I57" s="1" t="s">
         <v>194</v>
-      </c>
-      <c r="I57" s="1" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2866,111 +2961,117 @@
         <v>196</v>
       </c>
       <c r="C58" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E58" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="D58" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E58" s="1" t="s">
+      <c r="F58" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="F58" s="1" t="s">
+      <c r="G58" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H58" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="H58" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="I58" s="1" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B59" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="B59" s="1" t="s">
+      <c r="C59" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="C59" s="1" t="s">
-        <v>197</v>
-      </c>
       <c r="D59" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>203</v>
+        <v>204</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="H59" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I59" s="1" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="B60" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H60" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I60" s="1" t="s">
         <v>205</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E60" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="F60" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="G60" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H60" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I60" s="1" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B61" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="G61" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="H61" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I61" s="1" t="s">
         <v>205</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E61" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="F61" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="G61" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H61" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I61" s="1" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>210</v>
@@ -2982,7 +3083,7 @@
         <v>12</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="F62" s="1" t="s">
         <v>211</v>
@@ -2994,15 +3095,15 @@
         <v>16</v>
       </c>
       <c r="I62" s="1" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>12</v>
@@ -3011,24 +3112,24 @@
         <v>12</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
       <c r="H63" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I63" s="1" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>215</v>
@@ -3040,24 +3141,27 @@
         <v>12</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="F64" s="1" t="s">
         <v>216</v>
       </c>
+      <c r="G64" s="1" t="s">
+        <v>217</v>
+      </c>
       <c r="H64" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I64" s="1" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>12</v>
@@ -3066,102 +3170,114 @@
         <v>12</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>219</v>
+        <v>221</v>
+      </c>
+      <c r="G65" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="H65" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I65" s="1" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>197</v>
+        <v>12</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>222</v>
+        <v>224</v>
+      </c>
+      <c r="G66" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="H66" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I66" s="1" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>225</v>
+        <v>203</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>226</v>
+        <v>227</v>
+      </c>
+      <c r="G67" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="H67" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I67" s="1" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>12</v>
+        <v>202</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>198</v>
+        <v>230</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>229</v>
+        <v>231</v>
+      </c>
+      <c r="G68" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="H68" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I68" s="1" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>12</v>
@@ -3170,24 +3286,27 @@
         <v>12</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>232</v>
+        <v>234</v>
+      </c>
+      <c r="G69" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="H69" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I69" s="1" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>12</v>
@@ -3196,24 +3315,27 @@
         <v>12</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>235</v>
+        <v>237</v>
+      </c>
+      <c r="G70" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="H70" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I70" s="1" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>12</v>
@@ -3222,24 +3344,27 @@
         <v>12</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>238</v>
+        <v>240</v>
+      </c>
+      <c r="G71" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="H71" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I71" s="1" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>210</v>
+        <v>242</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>12</v>
@@ -3248,24 +3373,27 @@
         <v>12</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>240</v>
+        <v>243</v>
+      </c>
+      <c r="G72" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="H72" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I72" s="1" t="s">
-        <v>241</v>
+        <v>205</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>243</v>
+        <v>215</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>12</v>
@@ -3274,24 +3402,27 @@
         <v>12</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>244</v>
+        <v>203</v>
       </c>
       <c r="F73" s="1" t="s">
         <v>245</v>
       </c>
+      <c r="G73" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="H73" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I73" s="1" t="s">
-        <v>200</v>
+        <v>246</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>12</v>
@@ -3300,24 +3431,27 @@
         <v>12</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>198</v>
+        <v>249</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>248</v>
+        <v>250</v>
+      </c>
+      <c r="G74" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="H74" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I74" s="1" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>12</v>
@@ -3326,74 +3460,77 @@
         <v>12</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>251</v>
+        <v>253</v>
+      </c>
+      <c r="G75" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="H75" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I75" s="1" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="B76" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="F76" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="G76" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H76" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I76" s="1" t="s">
         <v>205</v>
-      </c>
-      <c r="C76" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D76" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E76" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="F76" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="G76" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H76" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I76" s="1" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>254</v>
+        <v>210</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>255</v>
+        <v>12</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>244</v>
+        <v>203</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>256</v>
+        <v>211</v>
       </c>
       <c r="G77" s="1" t="s">
-        <v>255</v>
+        <v>212</v>
       </c>
       <c r="H77" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I77" s="1" t="s">
-        <v>257</v>
+        <v>205</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3404,30 +3541,33 @@
         <v>259</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>12</v>
+        <v>260</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>198</v>
+        <v>249</v>
       </c>
       <c r="F78" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="G78" s="1" t="s">
         <v>260</v>
       </c>
       <c r="H78" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I78" s="1" t="s">
-        <v>200</v>
+        <v>262</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="C79" s="1" t="s">
         <v>12</v>
@@ -3436,180 +3576,201 @@
         <v>12</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>263</v>
+        <v>265</v>
+      </c>
+      <c r="G79" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="H79" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I79" s="1" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>266</v>
+        <v>12</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
+      </c>
+      <c r="G80" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="H80" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I80" s="1" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A81" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>265</v>
+        <v>270</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>267</v>
+        <v>272</v>
+      </c>
+      <c r="G81" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="H81" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I81" s="1" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A82" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="B82" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="B82" s="1" t="s">
-        <v>210</v>
-      </c>
       <c r="C82" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>12</v>
+        <v>274</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>240</v>
+        <v>272</v>
+      </c>
+      <c r="G82" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="H82" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I82" s="1" t="s">
-        <v>241</v>
+        <v>205</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A83" s="1" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>272</v>
+        <v>215</v>
       </c>
       <c r="C83" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>273</v>
+        <v>12</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>274</v>
+        <v>245</v>
+      </c>
+      <c r="G83" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="H83" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I83" s="1" t="s">
-        <v>200</v>
+        <v>246</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A84" s="1" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>231</v>
+        <v>277</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>232</v>
+        <v>279</v>
+      </c>
+      <c r="G84" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="H84" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I84" s="1" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A85" s="1" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>259</v>
+        <v>236</v>
       </c>
       <c r="C85" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>12</v>
+        <v>281</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>260</v>
+        <v>237</v>
+      </c>
+      <c r="G85" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="H85" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I85" s="1" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A86" s="1" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>259</v>
+        <v>264</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>12</v>
@@ -3618,24 +3779,27 @@
         <v>12</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>260</v>
+        <v>265</v>
+      </c>
+      <c r="G86" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="H86" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I86" s="1" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A87" s="1" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>280</v>
+        <v>264</v>
       </c>
       <c r="C87" s="1" t="s">
         <v>12</v>
@@ -3644,340 +3808,367 @@
         <v>12</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>281</v>
+        <v>265</v>
+      </c>
+      <c r="G87" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="H87" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I87" s="1" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A88" s="1" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>207</v>
+        <v>12</v>
       </c>
       <c r="D88" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>244</v>
+        <v>203</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="G88" s="1" t="s">
-        <v>285</v>
+        <v>12</v>
       </c>
       <c r="H88" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I88" s="1" t="s">
-        <v>257</v>
+        <v>205</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A89" s="1" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>12</v>
+        <v>212</v>
       </c>
       <c r="D89" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>198</v>
+        <v>249</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>288</v>
+        <v>289</v>
+      </c>
+      <c r="G89" s="1" t="s">
+        <v>290</v>
       </c>
       <c r="H89" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I89" s="1" t="s">
-        <v>200</v>
+        <v>262</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A90" s="1" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>287</v>
+        <v>292</v>
       </c>
       <c r="C90" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>290</v>
+        <v>12</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>288</v>
+        <v>293</v>
+      </c>
+      <c r="G90" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="H90" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I90" s="1" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A91" s="1" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>210</v>
+        <v>292</v>
       </c>
       <c r="C91" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>12</v>
+        <v>295</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>240</v>
+        <v>293</v>
+      </c>
+      <c r="G91" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="H91" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I91" s="1" t="s">
-        <v>241</v>
+        <v>205</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A92" s="1" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>293</v>
+        <v>215</v>
       </c>
       <c r="C92" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>294</v>
+        <v>12</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>295</v>
+        <v>245</v>
+      </c>
+      <c r="G92" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="H92" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I92" s="1" t="s">
-        <v>200</v>
+        <v>246</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A93" s="1" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="C93" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>299</v>
+        <v>300</v>
+      </c>
+      <c r="G93" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="H93" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I93" s="1" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A94" s="1" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="C94" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>303</v>
+        <v>304</v>
+      </c>
+      <c r="G94" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="H94" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I94" s="1" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A95" s="1" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>254</v>
+        <v>306</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>255</v>
+        <v>12</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>12</v>
+        <v>307</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>244</v>
+        <v>203</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>256</v>
+        <v>308</v>
       </c>
       <c r="G95" s="1" t="s">
-        <v>255</v>
+        <v>12</v>
       </c>
       <c r="H95" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I95" s="1" t="s">
-        <v>257</v>
+        <v>205</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A96" s="1" t="s">
-        <v>305</v>
+        <v>309</v>
       </c>
       <c r="B96" s="1" t="s">
         <v>259</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>12</v>
+        <v>260</v>
       </c>
       <c r="D96" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>198</v>
+        <v>249</v>
       </c>
       <c r="F96" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="G96" s="1" t="s">
         <v>260</v>
       </c>
       <c r="H96" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I96" s="1" t="s">
-        <v>200</v>
+        <v>262</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A97" s="1" t="s">
-        <v>306</v>
+        <v>310</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>307</v>
+        <v>264</v>
       </c>
       <c r="C97" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>308</v>
+        <v>12</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>309</v>
+        <v>265</v>
       </c>
       <c r="G97" s="1" t="s">
-        <v>207</v>
+        <v>12</v>
       </c>
       <c r="H97" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I97" s="1" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A98" s="1" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="C98" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>313</v>
+        <v>314</v>
+      </c>
+      <c r="G98" s="1" t="s">
+        <v>212</v>
       </c>
       <c r="H98" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I98" s="1" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A99" s="1" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>316</v>
+        <v>12</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>12</v>
+        <v>317</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="G99" s="1" t="s">
-        <v>316</v>
+        <v>12</v>
       </c>
       <c r="H99" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I99" s="1" t="s">
-        <v>318</v>
+        <v>205</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3988,33 +4179,33 @@
         <v>320</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>12</v>
+        <v>321</v>
       </c>
       <c r="D100" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="F100" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="G100" s="1" t="s">
         <v>321</v>
       </c>
-      <c r="G100" s="1" t="s">
-        <v>207</v>
-      </c>
       <c r="H100" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I100" s="1" t="s">
-        <v>200</v>
+        <v>323</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A101" s="1" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="C101" s="1" t="s">
         <v>12</v>
@@ -4023,27 +4214,27 @@
         <v>12</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="G101" s="1" t="s">
-        <v>207</v>
+        <v>212</v>
       </c>
       <c r="H101" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I101" s="1" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A102" s="1" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>320</v>
+        <v>328</v>
       </c>
       <c r="C102" s="1" t="s">
         <v>12</v>
@@ -4052,53 +4243,53 @@
         <v>12</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>321</v>
+        <v>329</v>
       </c>
       <c r="G102" s="1" t="s">
-        <v>207</v>
+        <v>212</v>
       </c>
       <c r="H102" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I102" s="1" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A103" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D103" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E103" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="F103" s="1" t="s">
         <v>326</v>
       </c>
-      <c r="B103" s="1" t="s">
-        <v>323</v>
-      </c>
-      <c r="C103" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D103" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E103" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="F103" s="1" t="s">
-        <v>324</v>
-      </c>
       <c r="G103" s="1" t="s">
-        <v>207</v>
+        <v>212</v>
       </c>
       <c r="H103" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I103" s="1" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A104" s="1" t="s">
-        <v>327</v>
+        <v>331</v>
       </c>
       <c r="B104" s="1" t="s">
         <v>328</v>
@@ -4110,25 +4301,28 @@
         <v>12</v>
       </c>
       <c r="E104" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="F104" s="1" t="s">
         <v>329</v>
       </c>
-      <c r="F104" s="1" t="s">
-        <v>330</v>
+      <c r="G104" s="1" t="s">
+        <v>212</v>
       </c>
       <c r="H104" s="1" t="s">
-        <v>331</v>
+        <v>16</v>
       </c>
       <c r="I104" s="1" t="s">
-        <v>332</v>
+        <v>205</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A105" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="B105" s="1" t="s">
         <v>333</v>
       </c>
-      <c r="B105" s="1" t="s">
-        <v>328</v>
-      </c>
       <c r="C105" s="1" t="s">
         <v>12</v>
       </c>
@@ -4136,16 +4330,19 @@
         <v>12</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>329</v>
+        <v>12</v>
       </c>
       <c r="F105" s="1" t="s">
-        <v>330</v>
+        <v>12</v>
+      </c>
+      <c r="G105" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="H105" s="1" t="s">
-        <v>331</v>
+        <v>16</v>
       </c>
       <c r="I105" s="1" t="s">
-        <v>332</v>
+        <v>205</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4153,7 +4350,7 @@
         <v>334</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>335</v>
+        <v>215</v>
       </c>
       <c r="C106" s="1" t="s">
         <v>12</v>
@@ -4162,24 +4359,27 @@
         <v>12</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>336</v>
+        <v>203</v>
       </c>
       <c r="F106" s="1" t="s">
-        <v>337</v>
+        <v>216</v>
+      </c>
+      <c r="G106" s="1" t="s">
+        <v>217</v>
       </c>
       <c r="H106" s="1" t="s">
-        <v>338</v>
+        <v>16</v>
       </c>
       <c r="I106" s="1" t="s">
-        <v>339</v>
+        <v>205</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A107" s="1" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>341</v>
+        <v>215</v>
       </c>
       <c r="C107" s="1" t="s">
         <v>12</v>
@@ -4188,24 +4388,27 @@
         <v>12</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>336</v>
+        <v>203</v>
       </c>
       <c r="F107" s="1" t="s">
-        <v>342</v>
+        <v>216</v>
+      </c>
+      <c r="G107" s="1" t="s">
+        <v>217</v>
       </c>
       <c r="H107" s="1" t="s">
-        <v>343</v>
+        <v>16</v>
       </c>
       <c r="I107" s="1" t="s">
-        <v>344</v>
+        <v>205</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A108" s="1" t="s">
-        <v>345</v>
+        <v>336</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>346</v>
+        <v>337</v>
       </c>
       <c r="C108" s="1" t="s">
         <v>12</v>
@@ -4214,24 +4417,27 @@
         <v>12</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>12</v>
+        <v>338</v>
       </c>
       <c r="F108" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="G108" s="1" t="s">
         <v>12</v>
       </c>
       <c r="H108" s="1" t="s">
-        <v>16</v>
+        <v>340</v>
       </c>
       <c r="I108" s="1" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A109" s="1" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>346</v>
+        <v>337</v>
       </c>
       <c r="C109" s="1" t="s">
         <v>12</v>
@@ -4240,51 +4446,57 @@
         <v>12</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>12</v>
+        <v>338</v>
       </c>
       <c r="F109" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="G109" s="1" t="s">
         <v>12</v>
       </c>
       <c r="H109" s="1" t="s">
-        <v>16</v>
+        <v>340</v>
       </c>
       <c r="I109" s="1" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A110" s="1" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="B110" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D110" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E110" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="F110" s="1" t="s">
         <v>346</v>
       </c>
-      <c r="C110" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D110" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E110" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F110" s="1" t="s">
+      <c r="G110" s="1" t="s">
         <v>12</v>
       </c>
       <c r="H110" s="1" t="s">
-        <v>16</v>
+        <v>347</v>
       </c>
       <c r="I110" s="1" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A111" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="B111" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="B111" s="1" t="s">
-        <v>346</v>
-      </c>
       <c r="C111" s="1" t="s">
         <v>12</v>
       </c>
@@ -4292,24 +4504,27 @@
         <v>12</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>12</v>
+        <v>345</v>
       </c>
       <c r="F111" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="G111" s="1" t="s">
         <v>12</v>
       </c>
       <c r="H111" s="1" t="s">
-        <v>16</v>
+        <v>352</v>
       </c>
       <c r="I111" s="1" t="s">
-        <v>347</v>
+        <v>353</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A112" s="1" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>346</v>
+        <v>355</v>
       </c>
       <c r="C112" s="1" t="s">
         <v>12</v>
@@ -4318,24 +4533,27 @@
         <v>12</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>12</v>
+        <v>118</v>
       </c>
       <c r="F112" s="1" t="s">
-        <v>12</v>
+        <v>355</v>
+      </c>
+      <c r="G112" s="1" t="s">
+        <v>356</v>
       </c>
       <c r="H112" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I112" s="1" t="s">
-        <v>347</v>
+        <v>357</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A113" s="1" t="s">
-        <v>352</v>
+        <v>358</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>346</v>
+        <v>359</v>
       </c>
       <c r="C113" s="1" t="s">
         <v>12</v>
@@ -4349,19 +4567,22 @@
       <c r="F113" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="G113" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="H113" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I113" s="1" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A114" s="1" t="s">
-        <v>353</v>
+        <v>361</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>354</v>
+        <v>359</v>
       </c>
       <c r="C114" s="1" t="s">
         <v>12</v>
@@ -4375,19 +4596,22 @@
       <c r="F114" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="G114" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="H114" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I114" s="1" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A115" s="1" t="s">
-        <v>356</v>
+        <v>362</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>354</v>
+        <v>359</v>
       </c>
       <c r="C115" s="1" t="s">
         <v>12</v>
@@ -4401,19 +4625,22 @@
       <c r="F115" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="G115" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="H115" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I115" s="1" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A116" s="1" t="s">
-        <v>357</v>
+        <v>363</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>354</v>
+        <v>359</v>
       </c>
       <c r="C116" s="1" t="s">
         <v>12</v>
@@ -4427,19 +4654,22 @@
       <c r="F116" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="G116" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="H116" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I116" s="1" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A117" s="1" t="s">
-        <v>358</v>
+        <v>364</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>354</v>
+        <v>359</v>
       </c>
       <c r="C117" s="1" t="s">
         <v>12</v>
@@ -4453,20 +4683,23 @@
       <c r="F117" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="G117" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="H117" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I117" s="1" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A118" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="B118" s="1" t="s">
         <v>359</v>
       </c>
-      <c r="B118" s="1" t="s">
-        <v>346</v>
-      </c>
       <c r="C118" s="1" t="s">
         <v>12</v>
       </c>
@@ -4479,37 +4712,188 @@
       <c r="F118" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="G118" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="H118" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I118" s="1" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A119" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D119" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E119" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F119" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G119" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H119" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I119" s="1" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A120" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="C120" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D120" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E120" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F120" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G120" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H120" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I120" s="1" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A121" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="C121" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D121" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E121" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F121" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G121" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H121" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I121" s="1" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A122" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="C122" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D122" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E122" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F122" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G122" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H122" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I122" s="1" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A123" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="C123" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D123" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E123" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F123" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G123" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H123" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I123" s="1" t="s">
         <v>360</v>
       </c>
-      <c r="B119" s="1" t="s">
-        <v>346</v>
-      </c>
-      <c r="C119" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D119" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E119" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F119" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H119" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I119" s="1" t="s">
-        <v>347</v>
+    </row>
+    <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A124" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="C124" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D124" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E124" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F124" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G124" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H124" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I124" s="1" t="s">
+        <v>360</v>
       </c>
     </row>
   </sheetData>

</xml_diff>